<commit_message>
nmv 12 05 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C1DE2E-1678-410D-A21E-4D5A01D45A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D85A64-C1CD-487A-94BB-B9B281A1BF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="15" r:id="rId1"/>
-    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId2"/>
+    <sheet name="5.2" sheetId="16" r:id="rId2"/>
+    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="177">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1570,6 +1571,198 @@
   </si>
   <si>
     <t>ord</t>
+  </si>
+  <si>
+    <t>5.2.1.1 :</t>
+  </si>
+  <si>
+    <t>5.2.1.2 :</t>
+  </si>
+  <si>
+    <t>5.2.1.3 :</t>
+  </si>
+  <si>
+    <t>5.2.1.4 :</t>
+  </si>
+  <si>
+    <t>5.2.1.5 :</t>
+  </si>
+  <si>
+    <t>5.2.1.6 :</t>
+  </si>
+  <si>
+    <t>5.2.1.7 :</t>
+  </si>
+  <si>
+    <t>5.2.2.1 :</t>
+  </si>
+  <si>
+    <t>5.2.2.2 :</t>
+  </si>
+  <si>
+    <t>5.2.2.3 :</t>
+  </si>
+  <si>
+    <t>5.2.2.4 :</t>
+  </si>
+  <si>
+    <t>5.2.2.5 :</t>
+  </si>
+  <si>
+    <t>5.2.2.6 :</t>
+  </si>
+  <si>
+    <t>5.2.3.1 :</t>
+  </si>
+  <si>
+    <t>5.2.3.2 :</t>
+  </si>
+  <si>
+    <t>5.2.3.3 :</t>
+  </si>
+  <si>
+    <t>5.2.3.4 :</t>
+  </si>
+  <si>
+    <t>5.2.3.5 :</t>
+  </si>
+  <si>
+    <t>5.2.3.6 :</t>
+  </si>
+  <si>
+    <t>5.2.3.7 :</t>
+  </si>
+  <si>
+    <t>5.2.4.1 :</t>
+  </si>
+  <si>
+    <t>5.2.4.2 :</t>
+  </si>
+  <si>
+    <t>5.2.4.3 :</t>
+  </si>
+  <si>
+    <t>5.2.4.4 :</t>
+  </si>
+  <si>
+    <t>5.2.5.1 :</t>
+  </si>
+  <si>
+    <t>5.2.5.2 :</t>
+  </si>
+  <si>
+    <t>5.2.5.3 :</t>
+  </si>
+  <si>
+    <t>5.2.5.4 :</t>
+  </si>
+  <si>
+    <t>5.2.5.5 :</t>
+  </si>
+  <si>
+    <t>5.2.5.6 :</t>
+  </si>
+  <si>
+    <t>5.2.6.1 :</t>
+  </si>
+  <si>
+    <t>5.2.6.2 :</t>
+  </si>
+  <si>
+    <t>5.2.6.3 :</t>
+  </si>
+  <si>
+    <t>5.2.6.4 :</t>
+  </si>
+  <si>
+    <t>5.2.6.5 :</t>
+  </si>
+  <si>
+    <t>5.2.7.1 :</t>
+  </si>
+  <si>
+    <t>5.2.7.2 :</t>
+  </si>
+  <si>
+    <t>5.2.7.3 :</t>
+  </si>
+  <si>
+    <t>5.2.7.4 :</t>
+  </si>
+  <si>
+    <t>5.2.7.5 :</t>
+  </si>
+  <si>
+    <t>5.2.8.1 :</t>
+  </si>
+  <si>
+    <t>5.2.8.2 :</t>
+  </si>
+  <si>
+    <t>5.2.8.3 :</t>
+  </si>
+  <si>
+    <t>5.2.8.4 :</t>
+  </si>
+  <si>
+    <t>5.2.8.5 :</t>
+  </si>
+  <si>
+    <t>5.2.8.6 :</t>
+  </si>
+  <si>
+    <t>5.2.8.7 :</t>
+  </si>
+  <si>
+    <t>5.2.9.1 :</t>
+  </si>
+  <si>
+    <t>5.2.9.2 :</t>
+  </si>
+  <si>
+    <t>5.2.9.3 :</t>
+  </si>
+  <si>
+    <t>5.2.9.4 :</t>
+  </si>
+  <si>
+    <t>5.2.9.5 :</t>
+  </si>
+  <si>
+    <t>5.2.9.6 :</t>
+  </si>
+  <si>
+    <t>5.2.10.1 :</t>
+  </si>
+  <si>
+    <t>5.2.10.2 :</t>
+  </si>
+  <si>
+    <t>5.2.10.3 :</t>
+  </si>
+  <si>
+    <t>5.2.10.4 :</t>
+  </si>
+  <si>
+    <t>5.2.10.5 :</t>
+  </si>
+  <si>
+    <t>5.2.10.6 :</t>
+  </si>
+  <si>
+    <t>5.2.10.7 :</t>
+  </si>
+  <si>
+    <t>5.2.11.1 :</t>
+  </si>
+  <si>
+    <t>5.2.11.2 :</t>
+  </si>
+  <si>
+    <t>5.2.12.1 :</t>
+  </si>
+  <si>
+    <t>5.2.12.2 :</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1855,7 +2048,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1865,6 +2058,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2147,9 +2341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P66" sqref="P66"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4605,6 +4799,2657 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193482FB-1B6C-43BB-9280-365C0A1517A1}">
+  <dimension ref="A1:L76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="33">
+        <v>11</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>3</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>39</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="33">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>5</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>46</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="33">
+        <v>9</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>1</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>3</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>40</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="33">
+        <v>3</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>4</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>47</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="33">
+        <v>7</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>2</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>43</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="33">
+        <v>8</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>3</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>42</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="33">
+        <v>3</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>1</v>
+      </c>
+      <c r="G8" s="33">
+        <v>4</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>37</v>
+      </c>
+      <c r="K8" s="33">
+        <v>42</v>
+      </c>
+      <c r="L8" s="33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="33">
+        <v>7</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>4</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>43</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="33">
+        <v>10</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>4</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>40</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="33">
+        <v>6</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>1</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>44</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="33">
+        <v>10</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>3</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>40</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="33">
+        <v>9</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>3</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>41</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>1</v>
+      </c>
+      <c r="G14" s="33">
+        <v>7</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>1</v>
+      </c>
+      <c r="J14" s="33">
+        <v>37</v>
+      </c>
+      <c r="K14" s="33">
+        <v>42</v>
+      </c>
+      <c r="L14" s="33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="33">
+        <v>9</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>41</v>
+      </c>
+      <c r="K15" s="33">
+        <v>50</v>
+      </c>
+      <c r="L15" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="33">
+        <v>5</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>1</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>6</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>44</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="33">
+        <v>3</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>3</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>0</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>44</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="33">
+        <v>7</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>3</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>5</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>40</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="33">
+        <v>6</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>6</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>38</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="33">
+        <v>13</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>6</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>37</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="33">
+        <v>12</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>1</v>
+      </c>
+      <c r="G21" s="33">
+        <v>5</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>34</v>
+      </c>
+      <c r="K21" s="33">
+        <v>47</v>
+      </c>
+      <c r="L21" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="33">
+        <v>4</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>1</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>8</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>45</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="33">
+        <v>11</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>2</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>39</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="33">
+        <v>15</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>6</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>35</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="33">
+        <v>15</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>1</v>
+      </c>
+      <c r="G25" s="33">
+        <v>6</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>32</v>
+      </c>
+      <c r="K25" s="33">
+        <v>48</v>
+      </c>
+      <c r="L25" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="33">
+        <v>6</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>3</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>44</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="33">
+        <v>9</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>2</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>41</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="33">
+        <v>9</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>41</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="33">
+        <v>8</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>2</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>9</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>40</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="33">
+        <v>14</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <v>2</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>36</v>
+      </c>
+      <c r="K30" s="33">
+        <v>50</v>
+      </c>
+      <c r="L30" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="33">
+        <v>12</v>
+      </c>
+      <c r="C31" s="33">
+        <v>1</v>
+      </c>
+      <c r="D31" s="33">
+        <v>2</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>1</v>
+      </c>
+      <c r="G31" s="33">
+        <v>9</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>61</v>
+      </c>
+      <c r="K31" s="33">
+        <v>75</v>
+      </c>
+      <c r="L31" s="33">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="33">
+        <v>10</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>6</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>40</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>4</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>44</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="33">
+        <v>12</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
+        <v>6</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>38</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="33">
+        <v>6</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>4</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>44</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="33">
+        <v>10</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>1</v>
+      </c>
+      <c r="G36" s="33">
+        <v>7</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>59</v>
+      </c>
+      <c r="K36" s="33">
+        <v>70</v>
+      </c>
+      <c r="L36" s="33">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="33">
+        <v>6</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
+      <c r="G37" s="33">
+        <v>1</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>44</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="33">
+        <v>6</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>5</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>44</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="33">
+        <v>7</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>2</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>8</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>41</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" s="33">
+        <v>4</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>3</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>3</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>43</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="33">
+        <v>12</v>
+      </c>
+      <c r="C41" s="33">
+        <v>1</v>
+      </c>
+      <c r="D41" s="33">
+        <v>1</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>1</v>
+      </c>
+      <c r="G41" s="33">
+        <v>4</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>42</v>
+      </c>
+      <c r="K41" s="33">
+        <v>55</v>
+      </c>
+      <c r="L41" s="33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="33">
+        <v>12</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>4</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>36</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="33">
+        <v>7</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <v>2</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>43</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="33">
+        <v>12</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
+      <c r="G44" s="33">
+        <v>3</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>38</v>
+      </c>
+      <c r="K44" s="33">
+        <v>50</v>
+      </c>
+      <c r="L44" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="33">
+        <v>6</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>0</v>
+      </c>
+      <c r="G45" s="33">
+        <v>6</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>44</v>
+      </c>
+      <c r="K45" s="33">
+        <v>50</v>
+      </c>
+      <c r="L45" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="33">
+        <v>7</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>1</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>43</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="33">
+        <v>7</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>0</v>
+      </c>
+      <c r="G47" s="33">
+        <v>4</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>43</v>
+      </c>
+      <c r="K47" s="33">
+        <v>50</v>
+      </c>
+      <c r="L47" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B48" s="33">
+        <v>5</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>0</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>1</v>
+      </c>
+      <c r="G48" s="33">
+        <v>9</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>71</v>
+      </c>
+      <c r="K48" s="33">
+        <v>77</v>
+      </c>
+      <c r="L48" s="33">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" s="33">
+        <v>2</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>0</v>
+      </c>
+      <c r="G49" s="33">
+        <v>5</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>48</v>
+      </c>
+      <c r="K49" s="33">
+        <v>50</v>
+      </c>
+      <c r="L49" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="33">
+        <v>9</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>0</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>0</v>
+      </c>
+      <c r="G50" s="33">
+        <v>4</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>41</v>
+      </c>
+      <c r="K50" s="33">
+        <v>50</v>
+      </c>
+      <c r="L50" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="33">
+        <v>11</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>0</v>
+      </c>
+      <c r="G51" s="33">
+        <v>4</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>39</v>
+      </c>
+      <c r="K51" s="33">
+        <v>50</v>
+      </c>
+      <c r="L51" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="33">
+        <v>4</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>0</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>0</v>
+      </c>
+      <c r="G52" s="33">
+        <v>3</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>46</v>
+      </c>
+      <c r="K52" s="33">
+        <v>50</v>
+      </c>
+      <c r="L52" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="33">
+        <v>7</v>
+      </c>
+      <c r="C53" s="33">
+        <v>0</v>
+      </c>
+      <c r="D53" s="33">
+        <v>0</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>0</v>
+      </c>
+      <c r="G53" s="33">
+        <v>6</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>43</v>
+      </c>
+      <c r="K53" s="33">
+        <v>50</v>
+      </c>
+      <c r="L53" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="33">
+        <v>4</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>1</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>1</v>
+      </c>
+      <c r="G54" s="33">
+        <v>2</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>38</v>
+      </c>
+      <c r="K54" s="33">
+        <v>44</v>
+      </c>
+      <c r="L54" s="33">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="33">
+        <v>0</v>
+      </c>
+      <c r="C55" s="33">
+        <v>0</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>0</v>
+      </c>
+      <c r="G55" s="33">
+        <v>5</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>0</v>
+      </c>
+      <c r="J55" s="33">
+        <v>50</v>
+      </c>
+      <c r="K55" s="33">
+        <v>50</v>
+      </c>
+      <c r="L55" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B56" s="33">
+        <v>5</v>
+      </c>
+      <c r="C56" s="33">
+        <v>0</v>
+      </c>
+      <c r="D56" s="33">
+        <v>0</v>
+      </c>
+      <c r="E56" s="33">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33">
+        <v>0</v>
+      </c>
+      <c r="G56" s="33">
+        <v>4</v>
+      </c>
+      <c r="H56" s="33">
+        <v>0</v>
+      </c>
+      <c r="I56" s="33">
+        <v>0</v>
+      </c>
+      <c r="J56" s="33">
+        <v>45</v>
+      </c>
+      <c r="K56" s="33">
+        <v>50</v>
+      </c>
+      <c r="L56" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="33">
+        <v>6</v>
+      </c>
+      <c r="C57" s="33">
+        <v>0</v>
+      </c>
+      <c r="D57" s="33">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
+        <v>0</v>
+      </c>
+      <c r="F57" s="33">
+        <v>0</v>
+      </c>
+      <c r="G57" s="33">
+        <v>3</v>
+      </c>
+      <c r="H57" s="33">
+        <v>0</v>
+      </c>
+      <c r="I57" s="33">
+        <v>0</v>
+      </c>
+      <c r="J57" s="33">
+        <v>44</v>
+      </c>
+      <c r="K57" s="33">
+        <v>50</v>
+      </c>
+      <c r="L57" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="33">
+        <v>7</v>
+      </c>
+      <c r="C58" s="33">
+        <v>0</v>
+      </c>
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33">
+        <v>0</v>
+      </c>
+      <c r="F58" s="33">
+        <v>0</v>
+      </c>
+      <c r="G58" s="33">
+        <v>2</v>
+      </c>
+      <c r="H58" s="33">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33">
+        <v>0</v>
+      </c>
+      <c r="J58" s="33">
+        <v>43</v>
+      </c>
+      <c r="K58" s="33">
+        <v>50</v>
+      </c>
+      <c r="L58" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="33">
+        <v>4</v>
+      </c>
+      <c r="C59" s="33">
+        <v>0</v>
+      </c>
+      <c r="D59" s="33">
+        <v>0</v>
+      </c>
+      <c r="E59" s="33">
+        <v>0</v>
+      </c>
+      <c r="F59" s="33">
+        <v>0</v>
+      </c>
+      <c r="G59" s="33">
+        <v>2</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="33">
+        <v>46</v>
+      </c>
+      <c r="K59" s="33">
+        <v>50</v>
+      </c>
+      <c r="L59" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="33">
+        <v>15</v>
+      </c>
+      <c r="C60" s="33">
+        <v>0</v>
+      </c>
+      <c r="D60" s="33">
+        <v>1</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0</v>
+      </c>
+      <c r="F60" s="33">
+        <v>0</v>
+      </c>
+      <c r="G60" s="33">
+        <v>5</v>
+      </c>
+      <c r="H60" s="33">
+        <v>0</v>
+      </c>
+      <c r="I60" s="33">
+        <v>0</v>
+      </c>
+      <c r="J60" s="33">
+        <v>34</v>
+      </c>
+      <c r="K60" s="33">
+        <v>50</v>
+      </c>
+      <c r="L60" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" s="33">
+        <v>8</v>
+      </c>
+      <c r="C61" s="33">
+        <v>0</v>
+      </c>
+      <c r="D61" s="33">
+        <v>0</v>
+      </c>
+      <c r="E61" s="33">
+        <v>0</v>
+      </c>
+      <c r="F61" s="33">
+        <v>1</v>
+      </c>
+      <c r="G61" s="33">
+        <v>2</v>
+      </c>
+      <c r="H61" s="33">
+        <v>0</v>
+      </c>
+      <c r="I61" s="33">
+        <v>0</v>
+      </c>
+      <c r="J61" s="33">
+        <v>26</v>
+      </c>
+      <c r="K61" s="33">
+        <v>35</v>
+      </c>
+      <c r="L61" s="33">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="33">
+        <v>11</v>
+      </c>
+      <c r="C62" s="33">
+        <v>3</v>
+      </c>
+      <c r="D62" s="33">
+        <v>0</v>
+      </c>
+      <c r="E62" s="33">
+        <v>0</v>
+      </c>
+      <c r="F62" s="33">
+        <v>8</v>
+      </c>
+      <c r="G62" s="33">
+        <v>0</v>
+      </c>
+      <c r="H62" s="33">
+        <v>0</v>
+      </c>
+      <c r="I62" s="33">
+        <v>0</v>
+      </c>
+      <c r="J62" s="33">
+        <v>34</v>
+      </c>
+      <c r="K62" s="33">
+        <v>50</v>
+      </c>
+      <c r="L62" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B63" s="33">
+        <v>5</v>
+      </c>
+      <c r="C63" s="33">
+        <v>1</v>
+      </c>
+      <c r="D63" s="33">
+        <v>0</v>
+      </c>
+      <c r="E63" s="33">
+        <v>0</v>
+      </c>
+      <c r="F63" s="33">
+        <v>4</v>
+      </c>
+      <c r="G63" s="33">
+        <v>1</v>
+      </c>
+      <c r="H63" s="33">
+        <v>0</v>
+      </c>
+      <c r="I63" s="33">
+        <v>0</v>
+      </c>
+      <c r="J63" s="33">
+        <v>22</v>
+      </c>
+      <c r="K63" s="33">
+        <v>30</v>
+      </c>
+      <c r="L63" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B64" s="33">
+        <v>6</v>
+      </c>
+      <c r="C64" s="33">
+        <v>0</v>
+      </c>
+      <c r="D64" s="33">
+        <v>0</v>
+      </c>
+      <c r="E64" s="33">
+        <v>0</v>
+      </c>
+      <c r="F64" s="33">
+        <v>7</v>
+      </c>
+      <c r="G64" s="33">
+        <v>3</v>
+      </c>
+      <c r="H64" s="33">
+        <v>0</v>
+      </c>
+      <c r="I64" s="33">
+        <v>0</v>
+      </c>
+      <c r="J64" s="33">
+        <v>37</v>
+      </c>
+      <c r="K64" s="33">
+        <v>50</v>
+      </c>
+      <c r="L64" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="33">
+        <v>2</v>
+      </c>
+      <c r="C65" s="33">
+        <v>0</v>
+      </c>
+      <c r="D65" s="33">
+        <v>0</v>
+      </c>
+      <c r="E65" s="33">
+        <v>0</v>
+      </c>
+      <c r="F65" s="33">
+        <v>5</v>
+      </c>
+      <c r="G65" s="33">
+        <v>0</v>
+      </c>
+      <c r="H65" s="33">
+        <v>0</v>
+      </c>
+      <c r="I65" s="33">
+        <v>0</v>
+      </c>
+      <c r="J65" s="33">
+        <v>23</v>
+      </c>
+      <c r="K65" s="33">
+        <v>30</v>
+      </c>
+      <c r="L65" s="33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="37">
+        <v>64</v>
+      </c>
+      <c r="B66" s="37">
+        <f>SUM(B2:B65)</f>
+        <v>490</v>
+      </c>
+      <c r="C66" s="37">
+        <f t="shared" ref="C66:L66" si="0">SUM(C2:C65)</f>
+        <v>6</v>
+      </c>
+      <c r="D66" s="37">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E66" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="37">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="G66" s="37">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+      <c r="H66" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J66" s="37">
+        <f t="shared" si="0"/>
+        <v>2647</v>
+      </c>
+      <c r="K66" s="37">
+        <f t="shared" si="0"/>
+        <v>3195</v>
+      </c>
+      <c r="L66" s="37">
+        <f t="shared" si="0"/>
+        <v>3709</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="38"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" t="s">
+        <v>106</v>
+      </c>
+      <c r="F67">
+        <f>G66</f>
+        <v>251</v>
+      </c>
+      <c r="J67">
+        <f>B66-C66</f>
+        <v>484</v>
+      </c>
+      <c r="K67" s="38"/>
+      <c r="L67" s="38"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="32"/>
+      <c r="E68" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68">
+        <f>B66</f>
+        <v>490</v>
+      </c>
+      <c r="J68">
+        <f>D66-E66</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69">
+        <v>28</v>
+      </c>
+      <c r="J69">
+        <f>F75</f>
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="J70" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F71" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J71">
+        <f>SUM(J67:J70)</f>
+        <v>3709</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f>SUM(F67:F71)</f>
+        <v>771</v>
+      </c>
+      <c r="J72" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>112</v>
+      </c>
+      <c r="F73">
+        <f>K66-F72</f>
+        <v>2424</v>
+      </c>
+      <c r="J73">
+        <f>J71-L66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F74" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f>F73+F72</f>
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f>F75-K66</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 24 05 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D85A64-C1CD-487A-94BB-B9B281A1BF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFFA99F-F8E8-4DFB-9784-354B36E5281A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="15" r:id="rId1"/>
     <sheet name="5.2" sheetId="16" r:id="rId2"/>
-    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId3"/>
+    <sheet name="5.3" sheetId="17" r:id="rId3"/>
+    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="225">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1763,6 +1764,150 @@
   </si>
   <si>
     <t>5.2.12.2 :</t>
+  </si>
+  <si>
+    <t>5.3.1.1 :</t>
+  </si>
+  <si>
+    <t>5.3.1.2 :</t>
+  </si>
+  <si>
+    <t>5.3.1.3 :</t>
+  </si>
+  <si>
+    <t>5.3.1.4 :</t>
+  </si>
+  <si>
+    <t>5.3.1.5 :</t>
+  </si>
+  <si>
+    <t>5.3.2.1 :</t>
+  </si>
+  <si>
+    <t>5.3.2.2 :</t>
+  </si>
+  <si>
+    <t>5.3.2.3 :</t>
+  </si>
+  <si>
+    <t>5.3.2.4 :</t>
+  </si>
+  <si>
+    <t>5.3.2.5 :</t>
+  </si>
+  <si>
+    <t>5.3.3.1 :</t>
+  </si>
+  <si>
+    <t>5.3.3.2 :</t>
+  </si>
+  <si>
+    <t>5.3.3.3 :</t>
+  </si>
+  <si>
+    <t>5.3.3.4 :</t>
+  </si>
+  <si>
+    <t>5.3.3.5 :</t>
+  </si>
+  <si>
+    <t>5.3.4.1 :</t>
+  </si>
+  <si>
+    <t>5.3.4.2 :</t>
+  </si>
+  <si>
+    <t>5.3.4.3 :</t>
+  </si>
+  <si>
+    <t>5.3.4.4 :</t>
+  </si>
+  <si>
+    <t>5.3.4.5 :</t>
+  </si>
+  <si>
+    <t>5.3.4.6 :</t>
+  </si>
+  <si>
+    <t>5.3.4.7 :</t>
+  </si>
+  <si>
+    <t>5.3.5.1 :</t>
+  </si>
+  <si>
+    <t>5.3.5.2 :</t>
+  </si>
+  <si>
+    <t>5.3.5.3 :</t>
+  </si>
+  <si>
+    <t>5.3.5.4 :</t>
+  </si>
+  <si>
+    <t>5.3.5.5 :</t>
+  </si>
+  <si>
+    <t>5.3.6.1 :</t>
+  </si>
+  <si>
+    <t>5.3.6.2 :</t>
+  </si>
+  <si>
+    <t>5.3.6.3 :</t>
+  </si>
+  <si>
+    <t>5.3.7.1 :</t>
+  </si>
+  <si>
+    <t>5.3.7.2 :</t>
+  </si>
+  <si>
+    <t>5.3.7.3 :</t>
+  </si>
+  <si>
+    <t>5.3.7.4 :</t>
+  </si>
+  <si>
+    <t>5.3.8.1 :</t>
+  </si>
+  <si>
+    <t>5.3.8.2 :</t>
+  </si>
+  <si>
+    <t>5.3.8.3 :</t>
+  </si>
+  <si>
+    <t>5.3.9.1 :</t>
+  </si>
+  <si>
+    <t>5.3.9.2 :</t>
+  </si>
+  <si>
+    <t>5.3.10.1 :</t>
+  </si>
+  <si>
+    <t>5.3.10.2 :</t>
+  </si>
+  <si>
+    <t>5.3.10.3 :</t>
+  </si>
+  <si>
+    <t>5.3.10.4 :</t>
+  </si>
+  <si>
+    <t>5.3.11.1 :</t>
+  </si>
+  <si>
+    <t>5.3.11.2 :</t>
+  </si>
+  <si>
+    <t>5.3.11.3 :</t>
+  </si>
+  <si>
+    <t>5.3.12.1 :</t>
+  </si>
+  <si>
+    <t>5.3.12.2 :</t>
   </si>
 </sst>
 </file>
@@ -1959,7 +2104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2058,7 +2203,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4802,9 +4946,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193482FB-1B6C-43BB-9280-365C0A1517A1}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L66"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67:K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7341,10 +7485,10 @@
       </c>
     </row>
     <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="38"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
       <c r="E67" t="s">
         <v>106</v>
       </c>
@@ -7356,8 +7500,8 @@
         <f>B66-C66</f>
         <v>484</v>
       </c>
-      <c r="K67" s="38"/>
-      <c r="L67" s="38"/>
+      <c r="K67" s="34"/>
+      <c r="L67" s="34"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="32"/>
@@ -7450,6 +7594,2044 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC17E510-A7CF-48B8-95B1-E6A35B35ABB9}">
+  <dimension ref="A1:L60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="33">
+        <v>2</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>3</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>48</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="33">
+        <v>9</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>1</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>3</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>40</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="33">
+        <v>13</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>5</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>37</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="33">
+        <v>8</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>4</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>3</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>38</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="33">
+        <v>6</v>
+      </c>
+      <c r="C6" s="33">
+        <v>1</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>4</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>49</v>
+      </c>
+      <c r="K6" s="33">
+        <v>55</v>
+      </c>
+      <c r="L6" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="33">
+        <v>7</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>3</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>4</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>40</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="33">
+        <v>12</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>2</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>3</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>36</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="33">
+        <v>9</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>4</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>41</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="33">
+        <v>8</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>4</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>42</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="33">
+        <v>7</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1</v>
+      </c>
+      <c r="G11" s="33">
+        <v>2</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>26</v>
+      </c>
+      <c r="K11" s="33">
+        <v>34</v>
+      </c>
+      <c r="L11" s="33">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="33">
+        <v>10</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>4</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>40</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="33">
+        <v>16</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>1</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>34</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="33">
+        <v>14</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>2</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>3</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>34</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" s="33">
+        <v>11</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>39</v>
+      </c>
+      <c r="K15" s="33">
+        <v>50</v>
+      </c>
+      <c r="L15" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="33">
+        <v>16</v>
+      </c>
+      <c r="C16" s="33">
+        <v>1</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>1</v>
+      </c>
+      <c r="G16" s="33">
+        <v>2</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>39</v>
+      </c>
+      <c r="K16" s="33">
+        <v>55</v>
+      </c>
+      <c r="L16" s="33">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B17" s="33">
+        <v>9</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>3</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>41</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18" s="33">
+        <v>10</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>40</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="33">
+        <v>8</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>42</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" s="33">
+        <v>16</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>1</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>34</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" s="33">
+        <v>12</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>1</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>38</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="33">
+        <v>7</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>4</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>43</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="33">
+        <v>8</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>1</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>1</v>
+      </c>
+      <c r="G23" s="33">
+        <v>9</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>54</v>
+      </c>
+      <c r="K23" s="33">
+        <v>64</v>
+      </c>
+      <c r="L23" s="33">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="33">
+        <v>7</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>4</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>43</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" s="33">
+        <v>8</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>2</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>3</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>40</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="33">
+        <v>11</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>4</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>39</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="33">
+        <v>7</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>2</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>43</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" s="33">
+        <v>15</v>
+      </c>
+      <c r="C28" s="33">
+        <v>1</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>1</v>
+      </c>
+      <c r="G28" s="33">
+        <v>2</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>28</v>
+      </c>
+      <c r="K28" s="33">
+        <v>43</v>
+      </c>
+      <c r="L28" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" s="33">
+        <v>12</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>0</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>38</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30" s="33">
+        <v>13</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <v>1</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>37</v>
+      </c>
+      <c r="K30" s="33">
+        <v>50</v>
+      </c>
+      <c r="L30" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" s="33">
+        <v>12</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>1</v>
+      </c>
+      <c r="G31" s="33">
+        <v>6</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>49</v>
+      </c>
+      <c r="K31" s="33">
+        <v>62</v>
+      </c>
+      <c r="L31" s="33">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="33">
+        <v>18</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>0</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>32</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33" s="33">
+        <v>8</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>6</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>41</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="B34" s="33">
+        <v>15</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>1</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
+        <v>4</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>34</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B35" s="33">
+        <v>22</v>
+      </c>
+      <c r="C35" s="33">
+        <v>1</v>
+      </c>
+      <c r="D35" s="33">
+        <v>2</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>1</v>
+      </c>
+      <c r="G35" s="33">
+        <v>7</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>48</v>
+      </c>
+      <c r="K35" s="33">
+        <v>72</v>
+      </c>
+      <c r="L35" s="33">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="33">
+        <v>2</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>0</v>
+      </c>
+      <c r="G36" s="33">
+        <v>6</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>48</v>
+      </c>
+      <c r="K36" s="33">
+        <v>50</v>
+      </c>
+      <c r="L36" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="33">
+        <v>9</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
+      <c r="G37" s="33">
+        <v>5</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>41</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38" s="33">
+        <v>12</v>
+      </c>
+      <c r="C38" s="33">
+        <v>1</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>1</v>
+      </c>
+      <c r="G38" s="33">
+        <v>3</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>39</v>
+      </c>
+      <c r="K38" s="33">
+        <v>51</v>
+      </c>
+      <c r="L38" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="33">
+        <v>11</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>1</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>1</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>38</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="33">
+        <v>10</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>1</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>1</v>
+      </c>
+      <c r="G40" s="33">
+        <v>4</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>42</v>
+      </c>
+      <c r="K40" s="33">
+        <v>54</v>
+      </c>
+      <c r="L40" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="33">
+        <v>12</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>4</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>38</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42" s="33">
+        <v>6</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>0</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>4</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>44</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="33">
+        <v>3</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <v>3</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>47</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44" s="33">
+        <v>6</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>1</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>1</v>
+      </c>
+      <c r="G44" s="33">
+        <v>3</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>41</v>
+      </c>
+      <c r="K44" s="33">
+        <v>49</v>
+      </c>
+      <c r="L44" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" s="33">
+        <v>7</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>0</v>
+      </c>
+      <c r="G45" s="33">
+        <v>1</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>43</v>
+      </c>
+      <c r="K45" s="33">
+        <v>50</v>
+      </c>
+      <c r="L45" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="33">
+        <v>4</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>5</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>46</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47" s="33">
+        <v>7</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>1</v>
+      </c>
+      <c r="G47" s="33">
+        <v>9</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>68</v>
+      </c>
+      <c r="K47" s="33">
+        <v>76</v>
+      </c>
+      <c r="L47" s="33">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="33">
+        <v>6</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>0</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
+      <c r="G48" s="33">
+        <v>3</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>44</v>
+      </c>
+      <c r="K48" s="33">
+        <v>50</v>
+      </c>
+      <c r="L48" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49" s="33">
+        <v>11</v>
+      </c>
+      <c r="C49" s="33">
+        <v>1</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>1</v>
+      </c>
+      <c r="G49" s="33">
+        <v>4</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>51</v>
+      </c>
+      <c r="K49" s="33">
+        <v>62</v>
+      </c>
+      <c r="L49" s="33">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="37">
+        <v>48</v>
+      </c>
+      <c r="B50" s="37">
+        <f>SUM(B2:B49)</f>
+        <v>472</v>
+      </c>
+      <c r="C50" s="37">
+        <f t="shared" ref="C50:L50" si="0">SUM(C2:C49)</f>
+        <v>6</v>
+      </c>
+      <c r="D50" s="37">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E50" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G50" s="37">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="H50" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="37">
+        <f t="shared" si="0"/>
+        <v>1977</v>
+      </c>
+      <c r="K50" s="37">
+        <f t="shared" si="0"/>
+        <v>2477</v>
+      </c>
+      <c r="L50" s="37">
+        <f t="shared" si="0"/>
+        <v>2965</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
+      <c r="E51" t="s">
+        <v>106</v>
+      </c>
+      <c r="F51">
+        <f>G50</f>
+        <v>162</v>
+      </c>
+      <c r="J51">
+        <f>B50-C50</f>
+        <v>466</v>
+      </c>
+      <c r="K51" s="34"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52">
+        <f>B50</f>
+        <v>472</v>
+      </c>
+      <c r="J52">
+        <f>D50-E50</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53">
+        <v>18</v>
+      </c>
+      <c r="J53">
+        <f>F59</f>
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>109</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="J54" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F55" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J55">
+        <f>SUM(J51:J54)</f>
+        <v>2965</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f>SUM(F51:F55)</f>
+        <v>656</v>
+      </c>
+      <c r="J56" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>112</v>
+      </c>
+      <c r="F57">
+        <f>K50-F56</f>
+        <v>1821</v>
+      </c>
+      <c r="J57">
+        <f>J55-L50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F58" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f>F57+F56</f>
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f>F59-K50</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 16 06 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFFA99F-F8E8-4DFB-9784-354B36E5281A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAA5828-0B49-4019-B9AD-CD76F9E623DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="15" r:id="rId1"/>
     <sheet name="5.2" sheetId="16" r:id="rId2"/>
     <sheet name="5.3" sheetId="17" r:id="rId3"/>
-    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId4"/>
+    <sheet name="5.4" sheetId="18" r:id="rId4"/>
+    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="284">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1909,6 +1910,183 @@
   <si>
     <t>5.3.12.2 :</t>
   </si>
+  <si>
+    <t>5.4.1.1 :</t>
+  </si>
+  <si>
+    <t>5.4.1.2 :</t>
+  </si>
+  <si>
+    <t>5.4.1.3 :</t>
+  </si>
+  <si>
+    <t>5.4.1.4 :</t>
+  </si>
+  <si>
+    <t>5.4.2.1 :</t>
+  </si>
+  <si>
+    <t>5.4.2.2 :</t>
+  </si>
+  <si>
+    <t>5.4.2.3 :</t>
+  </si>
+  <si>
+    <t>5.4.2.4 :</t>
+  </si>
+  <si>
+    <t>5.4.3.1 :</t>
+  </si>
+  <si>
+    <t>5.4.3.2 :</t>
+  </si>
+  <si>
+    <t>5.4.3.3 :</t>
+  </si>
+  <si>
+    <t>5.4.3.4 :</t>
+  </si>
+  <si>
+    <t>5.4.3.5 :</t>
+  </si>
+  <si>
+    <t>5.4.4.1 :</t>
+  </si>
+  <si>
+    <t>5.4.4.2 :</t>
+  </si>
+  <si>
+    <t>5.4.4.3 :</t>
+  </si>
+  <si>
+    <t>5.4.4.4 :</t>
+  </si>
+  <si>
+    <t>5.4.4.5 :</t>
+  </si>
+  <si>
+    <t>5.4.5.1 :</t>
+  </si>
+  <si>
+    <t>5.4.5.2 :</t>
+  </si>
+  <si>
+    <t>5.4.5.3 :</t>
+  </si>
+  <si>
+    <t>5.4.5.4 :</t>
+  </si>
+  <si>
+    <t>5.4.5.5 :</t>
+  </si>
+  <si>
+    <t>5.4.6.1 :</t>
+  </si>
+  <si>
+    <t>5.4.6.2 :</t>
+  </si>
+  <si>
+    <t>5.4.6.3 :</t>
+  </si>
+  <si>
+    <t>5.4.6.4 :</t>
+  </si>
+  <si>
+    <t>5.4.6.5 :</t>
+  </si>
+  <si>
+    <t>5.4.6.6 :</t>
+  </si>
+  <si>
+    <t>5.4.7.1 :</t>
+  </si>
+  <si>
+    <t>5.4.7.2 :</t>
+  </si>
+  <si>
+    <t>5.4.7.3 :</t>
+  </si>
+  <si>
+    <t>5.4.7.4 :</t>
+  </si>
+  <si>
+    <t>5.4.7.5 :</t>
+  </si>
+  <si>
+    <t>5.4.7.6 :</t>
+  </si>
+  <si>
+    <t>5.4.7.7 :</t>
+  </si>
+  <si>
+    <t>5.4.8.1 :</t>
+  </si>
+  <si>
+    <t>5.4.8.2 :</t>
+  </si>
+  <si>
+    <t>5.4.8.3 :</t>
+  </si>
+  <si>
+    <t>5.4.8.4 :</t>
+  </si>
+  <si>
+    <t>5.4.8.5 :</t>
+  </si>
+  <si>
+    <t>5.4.8.6 :</t>
+  </si>
+  <si>
+    <t>5.4.9.1 :</t>
+  </si>
+  <si>
+    <t>5.4.9.2 :</t>
+  </si>
+  <si>
+    <t>5.4.9.3 :</t>
+  </si>
+  <si>
+    <t>5.4.9.4 :</t>
+  </si>
+  <si>
+    <t>5.4.10.1 :</t>
+  </si>
+  <si>
+    <t>5.4.10.2 :</t>
+  </si>
+  <si>
+    <t>5.4.10.3 :</t>
+  </si>
+  <si>
+    <t>5.4.10.4 :</t>
+  </si>
+  <si>
+    <t>5.4.10.5 :</t>
+  </si>
+  <si>
+    <t>5.4.11.1 :</t>
+  </si>
+  <si>
+    <t>5.4.11.2 :</t>
+  </si>
+  <si>
+    <t>5.4.11.3 :</t>
+  </si>
+  <si>
+    <t>5.4.11.4 :</t>
+  </si>
+  <si>
+    <t>5.4.12.1 :</t>
+  </si>
+  <si>
+    <t>5.4.12.2 :</t>
+  </si>
+  <si>
+    <t>5.4.12.3 :</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
 </sst>
 </file>
 
@@ -2104,7 +2282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2202,6 +2380,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7597,9 +7778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC17E510-A7CF-48B8-95B1-E6A35B35ABB9}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L50"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51:K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9632,6 +9813,2424 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A771221C-D551-416E-9E70-872AB0613614}">
+  <dimension ref="A1:L70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="33">
+        <v>6</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>1</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>4</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>43</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="33">
+        <v>9</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>1</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>6</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>40</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="33">
+        <v>3</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>1</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>4</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>46</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="33">
+        <v>5</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>1</v>
+      </c>
+      <c r="G5" s="33">
+        <v>4</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>35</v>
+      </c>
+      <c r="K5" s="33">
+        <v>41</v>
+      </c>
+      <c r="L5" s="33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="33">
+        <v>7</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>5</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>43</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="33">
+        <v>7</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>1</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>43</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="33">
+        <v>10</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>3</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>39</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="33">
+        <v>6</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>2</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
+      <c r="G9" s="33">
+        <v>3</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>30</v>
+      </c>
+      <c r="K9" s="33">
+        <v>39</v>
+      </c>
+      <c r="L9" s="33">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="33">
+        <v>5</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>2</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>45</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="33">
+        <v>6</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>0</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>43</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="33">
+        <v>7</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>2</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>43</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="33">
+        <v>7</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>1</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>1</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>42</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="33">
+        <v>5</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>1</v>
+      </c>
+      <c r="G14" s="33">
+        <v>2</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>24</v>
+      </c>
+      <c r="K14" s="33">
+        <v>30</v>
+      </c>
+      <c r="L14" s="33">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="33">
+        <v>3</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>1</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>46</v>
+      </c>
+      <c r="K15" s="33">
+        <v>50</v>
+      </c>
+      <c r="L15" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" s="33">
+        <v>3</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>3</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>47</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="33">
+        <v>4</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>3</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>46</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="B18" s="33">
+        <v>5</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>1</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>1</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>44</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="33">
+        <v>6</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1</v>
+      </c>
+      <c r="G19" s="33">
+        <v>3</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>42</v>
+      </c>
+      <c r="K19" s="33">
+        <v>49</v>
+      </c>
+      <c r="L19" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="33">
+        <v>14</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>2</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>36</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="33">
+        <v>11</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>2</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>39</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="33">
+        <v>15</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>2</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>35</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="B23" s="33">
+        <v>12</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>4</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>38</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B24" s="33">
+        <v>5</v>
+      </c>
+      <c r="C24" s="33">
+        <v>1</v>
+      </c>
+      <c r="D24" s="33">
+        <v>2</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>1</v>
+      </c>
+      <c r="G24" s="33">
+        <v>4</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>33</v>
+      </c>
+      <c r="K24" s="33">
+        <v>40</v>
+      </c>
+      <c r="L24" s="33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" s="33">
+        <v>6</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>5</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>44</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="33">
+        <v>7</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>4</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>43</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="B27" s="33">
+        <v>10</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>2</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>2</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>38</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="B28" s="33">
+        <v>18</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>2</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>2</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>30</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="B29" s="33">
+        <v>8</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>4</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>42</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" s="33">
+        <v>11</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1</v>
+      </c>
+      <c r="G30" s="33">
+        <v>5</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>48</v>
+      </c>
+      <c r="K30" s="33">
+        <v>60</v>
+      </c>
+      <c r="L30" s="33">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B31" s="33">
+        <v>5</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <v>6</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>45</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="B32" s="33">
+        <v>8</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>3</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>42</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="B33" s="33">
+        <v>7</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>2</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>43</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="33">
+        <v>8</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
+        <v>3</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>42</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="B35" s="33">
+        <v>6</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>0</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>44</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="33">
+        <v>10</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>1</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>0</v>
+      </c>
+      <c r="G36" s="33">
+        <v>3</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>39</v>
+      </c>
+      <c r="K36" s="33">
+        <v>50</v>
+      </c>
+      <c r="L36" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="33">
+        <v>11</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>1</v>
+      </c>
+      <c r="G37" s="33">
+        <v>6</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>59</v>
+      </c>
+      <c r="K37" s="33">
+        <v>71</v>
+      </c>
+      <c r="L37" s="33">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>1</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>4</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>47</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" s="33">
+        <v>10</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>4</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>40</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B40" s="33">
+        <v>5</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>4</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>45</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="B41" s="33">
+        <v>6</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>1</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>3</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>43</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="B42" s="33">
+        <v>3</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>2</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>45</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B43" s="33">
+        <v>10</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>1</v>
+      </c>
+      <c r="G43" s="33">
+        <v>6</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>38</v>
+      </c>
+      <c r="K43" s="33">
+        <v>49</v>
+      </c>
+      <c r="L43" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B44" s="33">
+        <v>7</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>1</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
+      <c r="G44" s="33">
+        <v>4</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>42</v>
+      </c>
+      <c r="K44" s="33">
+        <v>50</v>
+      </c>
+      <c r="L44" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="B45" s="33">
+        <v>11</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>0</v>
+      </c>
+      <c r="G45" s="33">
+        <v>2</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>39</v>
+      </c>
+      <c r="K45" s="33">
+        <v>50</v>
+      </c>
+      <c r="L45" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="B46" s="33">
+        <v>7</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>3</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>3</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>40</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" s="33">
+        <v>4</v>
+      </c>
+      <c r="C47" s="33">
+        <v>1</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>1</v>
+      </c>
+      <c r="G47" s="33">
+        <v>5</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>48</v>
+      </c>
+      <c r="K47" s="33">
+        <v>52</v>
+      </c>
+      <c r="L47" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="B48" s="33">
+        <v>15</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>0</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>0</v>
+      </c>
+      <c r="G48" s="33">
+        <v>2</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>35</v>
+      </c>
+      <c r="K48" s="33">
+        <v>50</v>
+      </c>
+      <c r="L48" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B49" s="33">
+        <v>6</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>0</v>
+      </c>
+      <c r="G49" s="33">
+        <v>4</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>44</v>
+      </c>
+      <c r="K49" s="33">
+        <v>50</v>
+      </c>
+      <c r="L49" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="B50" s="33">
+        <v>8</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>1</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>0</v>
+      </c>
+      <c r="G50" s="33">
+        <v>7</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>41</v>
+      </c>
+      <c r="K50" s="33">
+        <v>50</v>
+      </c>
+      <c r="L50" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="B51" s="33">
+        <v>8</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>0</v>
+      </c>
+      <c r="G51" s="33">
+        <v>2</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>42</v>
+      </c>
+      <c r="K51" s="33">
+        <v>50</v>
+      </c>
+      <c r="L51" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B52" s="33">
+        <v>6</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>2</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>1</v>
+      </c>
+      <c r="G52" s="33">
+        <v>1</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>58</v>
+      </c>
+      <c r="K52" s="33">
+        <v>67</v>
+      </c>
+      <c r="L52" s="33">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="33">
+        <v>14</v>
+      </c>
+      <c r="C53" s="33">
+        <v>0</v>
+      </c>
+      <c r="D53" s="33">
+        <v>0</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>0</v>
+      </c>
+      <c r="G53" s="33">
+        <v>2</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>36</v>
+      </c>
+      <c r="K53" s="33">
+        <v>50</v>
+      </c>
+      <c r="L53" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="B54" s="33">
+        <v>9</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>0</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>0</v>
+      </c>
+      <c r="G54" s="33">
+        <v>6</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>41</v>
+      </c>
+      <c r="K54" s="33">
+        <v>50</v>
+      </c>
+      <c r="L54" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" s="33">
+        <v>9</v>
+      </c>
+      <c r="C55" s="33">
+        <v>0</v>
+      </c>
+      <c r="D55" s="33">
+        <v>1</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>0</v>
+      </c>
+      <c r="G55" s="33">
+        <v>2</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>1</v>
+      </c>
+      <c r="J55" s="33">
+        <v>40</v>
+      </c>
+      <c r="K55" s="33">
+        <v>50</v>
+      </c>
+      <c r="L55" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="B56" s="33">
+        <v>4</v>
+      </c>
+      <c r="C56" s="33">
+        <v>0</v>
+      </c>
+      <c r="D56" s="33">
+        <v>0</v>
+      </c>
+      <c r="E56" s="33">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33">
+        <v>1</v>
+      </c>
+      <c r="G56" s="33">
+        <v>5</v>
+      </c>
+      <c r="H56" s="33">
+        <v>0</v>
+      </c>
+      <c r="I56" s="33">
+        <v>0</v>
+      </c>
+      <c r="J56" s="33">
+        <v>43</v>
+      </c>
+      <c r="K56" s="33">
+        <v>48</v>
+      </c>
+      <c r="L56" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B57" s="33">
+        <v>11</v>
+      </c>
+      <c r="C57" s="33">
+        <v>0</v>
+      </c>
+      <c r="D57" s="33">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
+        <v>0</v>
+      </c>
+      <c r="F57" s="33">
+        <v>0</v>
+      </c>
+      <c r="G57" s="33">
+        <v>0</v>
+      </c>
+      <c r="H57" s="33">
+        <v>0</v>
+      </c>
+      <c r="I57" s="33">
+        <v>0</v>
+      </c>
+      <c r="J57" s="33">
+        <v>39</v>
+      </c>
+      <c r="K57" s="33">
+        <v>50</v>
+      </c>
+      <c r="L57" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B58" s="33">
+        <v>10</v>
+      </c>
+      <c r="C58" s="33">
+        <v>0</v>
+      </c>
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33">
+        <v>0</v>
+      </c>
+      <c r="F58" s="33">
+        <v>0</v>
+      </c>
+      <c r="G58" s="33">
+        <v>1</v>
+      </c>
+      <c r="H58" s="33">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33">
+        <v>0</v>
+      </c>
+      <c r="J58" s="33">
+        <v>40</v>
+      </c>
+      <c r="K58" s="33">
+        <v>50</v>
+      </c>
+      <c r="L58" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="B59" s="33">
+        <v>16</v>
+      </c>
+      <c r="C59" s="33">
+        <v>0</v>
+      </c>
+      <c r="D59" s="33">
+        <v>0</v>
+      </c>
+      <c r="E59" s="33">
+        <v>0</v>
+      </c>
+      <c r="F59" s="33">
+        <v>1</v>
+      </c>
+      <c r="G59" s="33">
+        <v>0</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="33">
+        <v>43</v>
+      </c>
+      <c r="K59" s="33">
+        <v>60</v>
+      </c>
+      <c r="L59" s="33">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="B60" s="37">
+        <f>SUM(B2:B59)</f>
+        <v>457</v>
+      </c>
+      <c r="C60" s="37">
+        <f t="shared" ref="C60:L60" si="0">SUM(C2:C59)</f>
+        <v>2</v>
+      </c>
+      <c r="D60" s="37">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E60" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G60" s="37">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="H60" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J60" s="37">
+        <f t="shared" si="0"/>
+        <v>2410</v>
+      </c>
+      <c r="K60" s="37">
+        <f t="shared" si="0"/>
+        <v>2906</v>
+      </c>
+      <c r="L60" s="37">
+        <f t="shared" si="0"/>
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="38"/>
+      <c r="E61" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61">
+        <f>G60</f>
+        <v>178</v>
+      </c>
+      <c r="J61">
+        <f>B60-C60</f>
+        <v>455</v>
+      </c>
+      <c r="K61" s="34"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>107</v>
+      </c>
+      <c r="F62">
+        <f>B60</f>
+        <v>457</v>
+      </c>
+      <c r="J62">
+        <f>D60-E60</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>108</v>
+      </c>
+      <c r="F63">
+        <v>24</v>
+      </c>
+      <c r="J63">
+        <f>F69</f>
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F65" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J65">
+        <f>SUM(J61:J64)</f>
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f>SUM(F61:F65)</f>
+        <v>663</v>
+      </c>
+      <c r="J66" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67">
+        <f>K60-F66</f>
+        <v>2243</v>
+      </c>
+      <c r="J67">
+        <f>J65-L60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F68" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f>F67+F66</f>
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>F69-K60</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 24 06 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAA5828-0B49-4019-B9AD-CD76F9E623DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB17120-336D-4556-9F21-73BB5CD8E9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="15" r:id="rId1"/>
     <sheet name="5.2" sheetId="16" r:id="rId2"/>
     <sheet name="5.3" sheetId="17" r:id="rId3"/>
     <sheet name="5.4" sheetId="18" r:id="rId4"/>
-    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId5"/>
+    <sheet name="5.5" sheetId="19" r:id="rId5"/>
+    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="347">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -2086,6 +2087,195 @@
   </si>
   <si>
     <t>58</t>
+  </si>
+  <si>
+    <t>5.5.1.1 :</t>
+  </si>
+  <si>
+    <t>5.5.1.2 :</t>
+  </si>
+  <si>
+    <t>5.5.1.3 :</t>
+  </si>
+  <si>
+    <t>5.5.1.4 :</t>
+  </si>
+  <si>
+    <t>5.5.1.5 :</t>
+  </si>
+  <si>
+    <t>5.5.1.6 :</t>
+  </si>
+  <si>
+    <t>5.5.1.7 :</t>
+  </si>
+  <si>
+    <t>5.5.2.1 :</t>
+  </si>
+  <si>
+    <t>5.5.2.2 :</t>
+  </si>
+  <si>
+    <t>5.5.2.3 :</t>
+  </si>
+  <si>
+    <t>5.5.2.4 :</t>
+  </si>
+  <si>
+    <t>5.5.2.5 :</t>
+  </si>
+  <si>
+    <t>5.5.2.6 :</t>
+  </si>
+  <si>
+    <t>5.5.2.7 :</t>
+  </si>
+  <si>
+    <t>5.5.3.1 :</t>
+  </si>
+  <si>
+    <t>5.5.3.2 :</t>
+  </si>
+  <si>
+    <t>5.5.3.3 :</t>
+  </si>
+  <si>
+    <t>5.5.4.1 :</t>
+  </si>
+  <si>
+    <t>5.5.4.2 :</t>
+  </si>
+  <si>
+    <t>5.5.4.3 :</t>
+  </si>
+  <si>
+    <t>5.5.4.4 :</t>
+  </si>
+  <si>
+    <t>5.5.5.1 :</t>
+  </si>
+  <si>
+    <t>5.5.5.2 :</t>
+  </si>
+  <si>
+    <t>5.5.5.3 :</t>
+  </si>
+  <si>
+    <t>5.5.5.4 :</t>
+  </si>
+  <si>
+    <t>5.5.6.1 :</t>
+  </si>
+  <si>
+    <t>5.5.6.2 :</t>
+  </si>
+  <si>
+    <t>5.5.6.3 :</t>
+  </si>
+  <si>
+    <t>5.5.7.1 :</t>
+  </si>
+  <si>
+    <t>5.5.7.2 :</t>
+  </si>
+  <si>
+    <t>5.5.7.3 :</t>
+  </si>
+  <si>
+    <t>5.5.7.4 :</t>
+  </si>
+  <si>
+    <t>5.5.7.5 :</t>
+  </si>
+  <si>
+    <t>5.5.8.1 :</t>
+  </si>
+  <si>
+    <t>5.5.8.2 :</t>
+  </si>
+  <si>
+    <t>5.5.8.3 :</t>
+  </si>
+  <si>
+    <t>5.5.9.1 :</t>
+  </si>
+  <si>
+    <t>5.5.9.2 :</t>
+  </si>
+  <si>
+    <t>5.5.9.3 :</t>
+  </si>
+  <si>
+    <t>5.5.9.4 :</t>
+  </si>
+  <si>
+    <t>5.5.9.5 :</t>
+  </si>
+  <si>
+    <t>5.5.10.1 :</t>
+  </si>
+  <si>
+    <t>5.5.10.2 :</t>
+  </si>
+  <si>
+    <t>5.5.10.3 :</t>
+  </si>
+  <si>
+    <t>5.5.10.4 :</t>
+  </si>
+  <si>
+    <t>5.5.10.5 :</t>
+  </si>
+  <si>
+    <t>5.5.10.6 :</t>
+  </si>
+  <si>
+    <t>5.5.10.7 :</t>
+  </si>
+  <si>
+    <t>5.5.11.1 :</t>
+  </si>
+  <si>
+    <t>5.5.12.1 :</t>
+  </si>
+  <si>
+    <t>5.5.13.1 :</t>
+  </si>
+  <si>
+    <t>5.5.14.1 :</t>
+  </si>
+  <si>
+    <t>5.5.15.1 :</t>
+  </si>
+  <si>
+    <t>5.5.16.1 :</t>
+  </si>
+  <si>
+    <t>5.5.17.1 :</t>
+  </si>
+  <si>
+    <t>5.5.18.1 :</t>
+  </si>
+  <si>
+    <t>5.5.19.1 :</t>
+  </si>
+  <si>
+    <t>5.5.20.1 :</t>
+  </si>
+  <si>
+    <t>5.5.21.1 :</t>
+  </si>
+  <si>
+    <t>5.5.22.1 :</t>
+  </si>
+  <si>
+    <t>5.5.23.1 :</t>
+  </si>
+  <si>
+    <t>5.5.24.1 :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2333  2727 3093</t>
   </si>
 </sst>
 </file>
@@ -9816,7 +10006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A771221C-D551-416E-9E70-872AB0613614}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:L60"/>
     </sheetView>
@@ -12231,6 +12421,2460 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64BAEC-8D94-4B07-A1DD-3D546E3471DD}">
+  <dimension ref="A1:L64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:L64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>37</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>42</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="L5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>46</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>44</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+      <c r="L7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>33</v>
+      </c>
+      <c r="K8">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>43</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>48</v>
+      </c>
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>47</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>46</v>
+      </c>
+      <c r="K12">
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>45</v>
+      </c>
+      <c r="K13">
+        <v>50</v>
+      </c>
+      <c r="L13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>46</v>
+      </c>
+      <c r="K14">
+        <v>50</v>
+      </c>
+      <c r="L14">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>36</v>
+      </c>
+      <c r="K15">
+        <v>40</v>
+      </c>
+      <c r="L15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>45</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>42</v>
+      </c>
+      <c r="K17">
+        <v>50</v>
+      </c>
+      <c r="L17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>57</v>
+      </c>
+      <c r="K18">
+        <v>74</v>
+      </c>
+      <c r="L18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>44</v>
+      </c>
+      <c r="K19">
+        <v>50</v>
+      </c>
+      <c r="L19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>43</v>
+      </c>
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="L20">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>37</v>
+      </c>
+      <c r="K21">
+        <v>50</v>
+      </c>
+      <c r="L21">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>57</v>
+      </c>
+      <c r="K22">
+        <v>68</v>
+      </c>
+      <c r="L22">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>305</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>43</v>
+      </c>
+      <c r="K23">
+        <v>50</v>
+      </c>
+      <c r="L23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>306</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>39</v>
+      </c>
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>307</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>34</v>
+      </c>
+      <c r="K25">
+        <v>50</v>
+      </c>
+      <c r="L25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>41</v>
+      </c>
+      <c r="K26">
+        <v>53</v>
+      </c>
+      <c r="L26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>309</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>49</v>
+      </c>
+      <c r="K27">
+        <v>50</v>
+      </c>
+      <c r="L27">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>34</v>
+      </c>
+      <c r="K28">
+        <v>50</v>
+      </c>
+      <c r="L28">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>311</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>62</v>
+      </c>
+      <c r="K29">
+        <v>66</v>
+      </c>
+      <c r="L29">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>312</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>42</v>
+      </c>
+      <c r="K30">
+        <v>50</v>
+      </c>
+      <c r="L30">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>47</v>
+      </c>
+      <c r="K31">
+        <v>50</v>
+      </c>
+      <c r="L31">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>314</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>47</v>
+      </c>
+      <c r="K32">
+        <v>50</v>
+      </c>
+      <c r="L32">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>315</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>47</v>
+      </c>
+      <c r="K33">
+        <v>50</v>
+      </c>
+      <c r="L33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>316</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>50</v>
+      </c>
+      <c r="K34">
+        <v>58</v>
+      </c>
+      <c r="L34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>317</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>43</v>
+      </c>
+      <c r="K35">
+        <v>50</v>
+      </c>
+      <c r="L35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>318</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>47</v>
+      </c>
+      <c r="K36">
+        <v>50</v>
+      </c>
+      <c r="L36">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>319</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>62</v>
+      </c>
+      <c r="K37">
+        <v>72</v>
+      </c>
+      <c r="L37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>320</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>48</v>
+      </c>
+      <c r="K38">
+        <v>50</v>
+      </c>
+      <c r="L38">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>321</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>46</v>
+      </c>
+      <c r="K39">
+        <v>50</v>
+      </c>
+      <c r="L39">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>322</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>42</v>
+      </c>
+      <c r="K40">
+        <v>50</v>
+      </c>
+      <c r="L40">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>323</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>43</v>
+      </c>
+      <c r="K41">
+        <v>50</v>
+      </c>
+      <c r="L41">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>324</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>25</v>
+      </c>
+      <c r="K42">
+        <v>32</v>
+      </c>
+      <c r="L42">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>325</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>47</v>
+      </c>
+      <c r="K43">
+        <v>50</v>
+      </c>
+      <c r="L43">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>326</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>40</v>
+      </c>
+      <c r="K44">
+        <v>50</v>
+      </c>
+      <c r="L44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>327</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>46</v>
+      </c>
+      <c r="K45">
+        <v>50</v>
+      </c>
+      <c r="L45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>328</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>47</v>
+      </c>
+      <c r="K46">
+        <v>50</v>
+      </c>
+      <c r="L46">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>329</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>40</v>
+      </c>
+      <c r="K47">
+        <v>50</v>
+      </c>
+      <c r="L47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>330</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>39</v>
+      </c>
+      <c r="K48">
+        <v>50</v>
+      </c>
+      <c r="L48">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>331</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>45</v>
+      </c>
+      <c r="K49">
+        <v>50</v>
+      </c>
+      <c r="L49">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>332</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>24</v>
+      </c>
+      <c r="K50">
+        <v>28</v>
+      </c>
+      <c r="L50">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>19</v>
+      </c>
+      <c r="K51">
+        <v>23</v>
+      </c>
+      <c r="L51">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>334</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>16</v>
+      </c>
+      <c r="K52">
+        <v>19</v>
+      </c>
+      <c r="L52">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>335</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>12</v>
+      </c>
+      <c r="K53">
+        <v>18</v>
+      </c>
+      <c r="L53">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>336</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>14</v>
+      </c>
+      <c r="K54">
+        <v>18</v>
+      </c>
+      <c r="L54">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>337</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>17</v>
+      </c>
+      <c r="K55">
+        <v>18</v>
+      </c>
+      <c r="L55">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>338</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>13</v>
+      </c>
+      <c r="K56">
+        <v>18</v>
+      </c>
+      <c r="L56">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>339</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>15</v>
+      </c>
+      <c r="K57">
+        <v>18</v>
+      </c>
+      <c r="L57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>340</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>17</v>
+      </c>
+      <c r="K58">
+        <v>20</v>
+      </c>
+      <c r="L58">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>341</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>14</v>
+      </c>
+      <c r="K59">
+        <v>18</v>
+      </c>
+      <c r="L59">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>342</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>15</v>
+      </c>
+      <c r="K60">
+        <v>18</v>
+      </c>
+      <c r="L60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>343</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>15</v>
+      </c>
+      <c r="K61">
+        <v>22</v>
+      </c>
+      <c r="L61">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>344</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>9</v>
+      </c>
+      <c r="K62">
+        <v>16</v>
+      </c>
+      <c r="L62">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>345</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>15</v>
+      </c>
+      <c r="K63">
+        <v>22</v>
+      </c>
+      <c r="L63">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="32">
+        <v>2.5833333333333335</v>
+      </c>
+      <c r="C64">
+        <v>354</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <v>15</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>28</v>
+      </c>
+      <c r="H64">
+        <v>133</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+      <c r="K64" t="s">
+        <v>346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>
@@ -12753,7 +15397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" ht="132" x14ac:dyDescent="0.4">
       <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
@@ -12775,7 +15419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" ht="115.5" x14ac:dyDescent="0.4">
       <c r="B28" s="10" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
nmv 02 07 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB17120-336D-4556-9F21-73BB5CD8E9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0CE85-DEF7-48A4-92C2-0F359A06192C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="347">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -2275,7 +2275,7 @@
     <t>5.5.24.1 :</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2333  2727 3093</t>
+    <t>62</t>
   </si>
 </sst>
 </file>
@@ -2472,7 +2472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2574,6 +2574,7 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10007,8 +10008,8 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L60"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61:J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12422,11 +12423,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64BAEC-8D94-4B07-A1DD-3D546E3471DD}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:L64"/>
+      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12481,2392 +12482,2513 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="33">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
         <v>2</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
         <v>40</v>
       </c>
-      <c r="K2">
-        <v>50</v>
-      </c>
-      <c r="L2">
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="33">
+        <v>10</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>3</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>6</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>37</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="33">
+        <v>5</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>2</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>45</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="33">
+        <v>8</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>2</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>42</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" s="33">
+        <v>4</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>46</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" s="33">
+        <v>5</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>4</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>44</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8" s="33">
+        <v>4</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>1</v>
+      </c>
+      <c r="G8" s="33">
+        <v>2</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>33</v>
+      </c>
+      <c r="K8" s="33">
+        <v>38</v>
+      </c>
+      <c r="L8" s="33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9" s="33">
+        <v>7</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>3</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>43</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" s="33">
+        <v>2</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>0</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>48</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11" s="33">
+        <v>3</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>4</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>47</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12" s="33">
+        <v>4</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>4</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>46</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13" s="33">
+        <v>5</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>7</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>45</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>6</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>46</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15" s="33">
+        <v>3</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
+      <c r="G15" s="33">
+        <v>4</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>36</v>
+      </c>
+      <c r="K15" s="33">
+        <v>40</v>
+      </c>
+      <c r="L15" s="33">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16" s="33">
+        <v>5</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>2</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>2</v>
+      </c>
+      <c r="J16" s="33">
+        <v>45</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="33">
+        <v>8</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>0</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>2</v>
+      </c>
+      <c r="J17" s="33">
+        <v>42</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18" s="33">
+        <v>15</v>
+      </c>
+      <c r="C18" s="33">
+        <v>1</v>
+      </c>
+      <c r="D18" s="33">
+        <v>2</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>1</v>
+      </c>
+      <c r="G18" s="33">
+        <v>4</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>57</v>
+      </c>
+      <c r="K18" s="33">
+        <v>74</v>
+      </c>
+      <c r="L18" s="33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" s="33">
+        <v>5</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>1</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>6</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>44</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="B20" s="33">
+        <v>4</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>3</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>4</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>43</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" s="33">
+        <v>12</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>1</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>0</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>37</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22" s="33">
+        <v>10</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>1</v>
+      </c>
+      <c r="G22" s="33">
+        <v>3</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>57</v>
+      </c>
+      <c r="K22" s="33">
+        <v>68</v>
+      </c>
+      <c r="L22" s="33">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B23" s="33">
+        <v>7</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>2</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>43</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="B24" s="33">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>6</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>39</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="B25" s="33">
+        <v>15</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>1</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>6</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>34</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="B26" s="33">
+        <v>11</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>1</v>
+      </c>
+      <c r="G26" s="33">
+        <v>3</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>41</v>
+      </c>
+      <c r="K26" s="33">
+        <v>53</v>
+      </c>
+      <c r="L26" s="33">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="B27" s="33">
+        <v>1</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0</v>
+      </c>
+      <c r="G27" s="33">
+        <v>3</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>49</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" s="33">
+        <v>15</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>1</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>34</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B29" s="33">
+        <v>3</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>1</v>
+      </c>
+      <c r="G29" s="33">
+        <v>5</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>62</v>
+      </c>
+      <c r="K29" s="33">
+        <v>66</v>
+      </c>
+      <c r="L29" s="33">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="B30" s="33">
+        <v>8</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <v>3</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>42</v>
+      </c>
+      <c r="K30" s="33">
+        <v>50</v>
+      </c>
+      <c r="L30" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31" s="33">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>1</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <v>5</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>47</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="B32" s="33">
+        <v>3</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>3</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>47</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="B33" s="33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>3</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>47</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="B34" s="33">
+        <v>5</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>3</v>
+      </c>
+      <c r="G34" s="33">
+        <v>2</v>
+      </c>
+      <c r="H34" s="33">
+        <v>1</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>50</v>
+      </c>
+      <c r="K34" s="33">
+        <v>58</v>
+      </c>
+      <c r="L34" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B35" s="33">
+        <v>7</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>3</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>43</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="B36" s="33">
+        <v>3</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>0</v>
+      </c>
+      <c r="G36" s="33">
+        <v>4</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>47</v>
+      </c>
+      <c r="K36" s="33">
+        <v>50</v>
+      </c>
+      <c r="L36" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B37" s="33">
+        <v>9</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>1</v>
+      </c>
+      <c r="G37" s="33">
+        <v>4</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>62</v>
+      </c>
+      <c r="K37" s="33">
+        <v>72</v>
+      </c>
+      <c r="L37" s="33">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>2</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>48</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B39" s="33">
+        <v>4</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>2</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>46</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B40" s="33">
+        <v>8</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>1</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>42</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="B41" s="33">
+        <v>7</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>1</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>43</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B42" s="33">
+        <v>7</v>
+      </c>
+      <c r="C42" s="33">
+        <v>1</v>
+      </c>
+      <c r="D42" s="33">
+        <v>0</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>1</v>
+      </c>
+      <c r="G42" s="33">
+        <v>0</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>25</v>
+      </c>
+      <c r="K42" s="33">
+        <v>32</v>
+      </c>
+      <c r="L42" s="33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="B43" s="33">
+        <v>3</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <v>0</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>47</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B44" s="33">
+        <v>10</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>0</v>
+      </c>
+      <c r="G44" s="33">
+        <v>0</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>40</v>
+      </c>
+      <c r="K44" s="33">
+        <v>50</v>
+      </c>
+      <c r="L44" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="B45" s="33">
+        <v>4</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>0</v>
+      </c>
+      <c r="G45" s="33">
+        <v>1</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>46</v>
+      </c>
+      <c r="K45" s="33">
+        <v>50</v>
+      </c>
+      <c r="L45" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="B46" s="33">
+        <v>3</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>0</v>
+      </c>
+      <c r="G46" s="33">
+        <v>0</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>47</v>
+      </c>
+      <c r="K46" s="33">
+        <v>50</v>
+      </c>
+      <c r="L46" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="B47" s="33">
+        <v>9</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>1</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>0</v>
+      </c>
+      <c r="G47" s="33">
+        <v>0</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>40</v>
+      </c>
+      <c r="K47" s="33">
+        <v>50</v>
+      </c>
+      <c r="L47" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="B48" s="33">
+        <v>9</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>0</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>2</v>
+      </c>
+      <c r="G48" s="33">
+        <v>4</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>39</v>
+      </c>
+      <c r="K48" s="33">
+        <v>50</v>
+      </c>
+      <c r="L48" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="B49" s="33">
+        <v>4</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>1</v>
+      </c>
+      <c r="G49" s="33">
+        <v>1</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>45</v>
+      </c>
+      <c r="K49" s="33">
+        <v>50</v>
+      </c>
+      <c r="L49" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="B50" s="33">
+        <v>3</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>0</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>1</v>
+      </c>
+      <c r="G50" s="33">
+        <v>0</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>24</v>
+      </c>
+      <c r="K50" s="33">
+        <v>28</v>
+      </c>
+      <c r="L50" s="33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51" s="33">
+        <v>3</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>1</v>
+      </c>
+      <c r="G51" s="33">
+        <v>0</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>19</v>
+      </c>
+      <c r="K51" s="33">
+        <v>23</v>
+      </c>
+      <c r="L51" s="33">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="B52" s="33">
+        <v>2</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>0</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>1</v>
+      </c>
+      <c r="G52" s="33">
+        <v>0</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>16</v>
+      </c>
+      <c r="K52" s="33">
+        <v>19</v>
+      </c>
+      <c r="L52" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="B53" s="33">
+        <v>5</v>
+      </c>
+      <c r="C53" s="33">
+        <v>0</v>
+      </c>
+      <c r="D53" s="33">
+        <v>0</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>1</v>
+      </c>
+      <c r="G53" s="33">
+        <v>0</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>12</v>
+      </c>
+      <c r="K53" s="33">
+        <v>18</v>
+      </c>
+      <c r="L53" s="33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="B54" s="33">
+        <v>3</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>0</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>1</v>
+      </c>
+      <c r="G54" s="33">
+        <v>0</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>14</v>
+      </c>
+      <c r="K54" s="33">
+        <v>18</v>
+      </c>
+      <c r="L54" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="B55" s="33">
+        <v>0</v>
+      </c>
+      <c r="C55" s="33">
+        <v>0</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>1</v>
+      </c>
+      <c r="G55" s="33">
+        <v>0</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>0</v>
+      </c>
+      <c r="J55" s="33">
+        <v>17</v>
+      </c>
+      <c r="K55" s="33">
+        <v>18</v>
+      </c>
+      <c r="L55" s="33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="B56" s="33">
+        <v>4</v>
+      </c>
+      <c r="C56" s="33">
+        <v>0</v>
+      </c>
+      <c r="D56" s="33">
+        <v>0</v>
+      </c>
+      <c r="E56" s="33">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33">
+        <v>1</v>
+      </c>
+      <c r="G56" s="33">
+        <v>0</v>
+      </c>
+      <c r="H56" s="33">
+        <v>0</v>
+      </c>
+      <c r="I56" s="33">
+        <v>0</v>
+      </c>
+      <c r="J56" s="33">
+        <v>13</v>
+      </c>
+      <c r="K56" s="33">
+        <v>18</v>
+      </c>
+      <c r="L56" s="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B57" s="33">
+        <v>2</v>
+      </c>
+      <c r="C57" s="33">
+        <v>0</v>
+      </c>
+      <c r="D57" s="33">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
+        <v>0</v>
+      </c>
+      <c r="F57" s="33">
+        <v>1</v>
+      </c>
+      <c r="G57" s="33">
+        <v>0</v>
+      </c>
+      <c r="H57" s="33">
+        <v>0</v>
+      </c>
+      <c r="I57" s="33">
+        <v>0</v>
+      </c>
+      <c r="J57" s="33">
+        <v>15</v>
+      </c>
+      <c r="K57" s="33">
+        <v>18</v>
+      </c>
+      <c r="L57" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B58" s="33">
+        <v>2</v>
+      </c>
+      <c r="C58" s="33">
+        <v>0</v>
+      </c>
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33">
+        <v>0</v>
+      </c>
+      <c r="F58" s="33">
+        <v>1</v>
+      </c>
+      <c r="G58" s="33">
+        <v>0</v>
+      </c>
+      <c r="H58" s="33">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33">
+        <v>0</v>
+      </c>
+      <c r="J58" s="33">
+        <v>17</v>
+      </c>
+      <c r="K58" s="33">
+        <v>20</v>
+      </c>
+      <c r="L58" s="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="B59" s="33">
+        <v>4</v>
+      </c>
+      <c r="C59" s="33">
+        <v>1</v>
+      </c>
+      <c r="D59" s="33">
+        <v>0</v>
+      </c>
+      <c r="E59" s="33">
+        <v>0</v>
+      </c>
+      <c r="F59" s="33">
+        <v>1</v>
+      </c>
+      <c r="G59" s="33">
+        <v>0</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="33">
+        <v>14</v>
+      </c>
+      <c r="K59" s="33">
+        <v>18</v>
+      </c>
+      <c r="L59" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="B60" s="33">
+        <v>2</v>
+      </c>
+      <c r="C60" s="33">
+        <v>0</v>
+      </c>
+      <c r="D60" s="33">
+        <v>0</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0</v>
+      </c>
+      <c r="F60" s="33">
+        <v>1</v>
+      </c>
+      <c r="G60" s="33">
+        <v>0</v>
+      </c>
+      <c r="H60" s="33">
+        <v>0</v>
+      </c>
+      <c r="I60" s="33">
+        <v>0</v>
+      </c>
+      <c r="J60" s="33">
+        <v>15</v>
+      </c>
+      <c r="K60" s="33">
+        <v>18</v>
+      </c>
+      <c r="L60" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="B61" s="33">
         <v>6</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>37</v>
-      </c>
-      <c r="K3">
-        <v>50</v>
-      </c>
-      <c r="L3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>286</v>
-      </c>
-      <c r="B4">
+      <c r="C61" s="33">
+        <v>0</v>
+      </c>
+      <c r="D61" s="33">
+        <v>0</v>
+      </c>
+      <c r="E61" s="33">
+        <v>0</v>
+      </c>
+      <c r="F61" s="33">
+        <v>1</v>
+      </c>
+      <c r="G61" s="33">
+        <v>0</v>
+      </c>
+      <c r="H61" s="33">
+        <v>0</v>
+      </c>
+      <c r="I61" s="33">
+        <v>0</v>
+      </c>
+      <c r="J61" s="33">
+        <v>15</v>
+      </c>
+      <c r="K61" s="33">
+        <v>22</v>
+      </c>
+      <c r="L61" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="B62" s="33">
+        <v>6</v>
+      </c>
+      <c r="C62" s="33">
+        <v>0</v>
+      </c>
+      <c r="D62" s="33">
+        <v>0</v>
+      </c>
+      <c r="E62" s="33">
+        <v>0</v>
+      </c>
+      <c r="F62" s="33">
+        <v>1</v>
+      </c>
+      <c r="G62" s="33">
+        <v>0</v>
+      </c>
+      <c r="H62" s="33">
+        <v>0</v>
+      </c>
+      <c r="I62" s="33">
+        <v>0</v>
+      </c>
+      <c r="J62" s="33">
+        <v>9</v>
+      </c>
+      <c r="K62" s="33">
+        <v>16</v>
+      </c>
+      <c r="L62" s="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="B63" s="33">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>45</v>
-      </c>
-      <c r="K4">
-        <v>50</v>
-      </c>
-      <c r="L4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>42</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
-      </c>
-      <c r="L5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>288</v>
-      </c>
-      <c r="B6">
+      <c r="C63" s="33">
+        <v>0</v>
+      </c>
+      <c r="D63" s="33">
+        <v>1</v>
+      </c>
+      <c r="E63" s="33">
+        <v>0</v>
+      </c>
+      <c r="F63" s="33">
+        <v>1</v>
+      </c>
+      <c r="G63" s="33">
+        <v>0</v>
+      </c>
+      <c r="H63" s="33">
+        <v>0</v>
+      </c>
+      <c r="I63" s="33">
+        <v>0</v>
+      </c>
+      <c r="J63" s="33">
+        <v>15</v>
+      </c>
+      <c r="K63" s="33">
+        <v>22</v>
+      </c>
+      <c r="L63" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="37" t="s">
+        <v>346</v>
+      </c>
+      <c r="B64" s="37">
+        <f>SUM(B2:B63)</f>
+        <v>353</v>
+      </c>
+      <c r="C64" s="37">
+        <f>SUM(C2:C63)</f>
+        <v>3</v>
+      </c>
+      <c r="D64" s="37">
+        <f t="shared" ref="D64:L64" si="0">SUM(D2:D63)</f>
+        <v>16</v>
+      </c>
+      <c r="E64" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="37">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G64" s="37">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="H64" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I64" s="37">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>46</v>
-      </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
-      <c r="L6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B7">
+      <c r="J64" s="37">
+        <f t="shared" si="0"/>
+        <v>2333</v>
+      </c>
+      <c r="K64" s="37">
+        <f t="shared" si="0"/>
+        <v>2727</v>
+      </c>
+      <c r="L64" s="37">
+        <f t="shared" si="0"/>
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="39"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" t="s">
+        <v>106</v>
+      </c>
+      <c r="F65">
+        <f>G64</f>
+        <v>133</v>
+      </c>
+      <c r="J65">
+        <f>B64-C64</f>
+        <v>350</v>
+      </c>
+      <c r="K65" s="39"/>
+      <c r="L65" s="39"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
+      <c r="E66" t="s">
+        <v>107</v>
+      </c>
+      <c r="F66">
+        <f>B64</f>
+        <v>353</v>
+      </c>
+      <c r="J66">
+        <f>D64-E64</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>108</v>
+      </c>
+      <c r="F67">
+        <v>11</v>
+      </c>
+      <c r="J67">
+        <f>F73</f>
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>109</v>
+      </c>
+      <c r="F68">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>44</v>
-      </c>
-      <c r="K7">
-        <v>50</v>
-      </c>
-      <c r="L7">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>290</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>33</v>
-      </c>
-      <c r="K8">
-        <v>38</v>
-      </c>
-      <c r="L8">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>43</v>
-      </c>
-      <c r="K9">
-        <v>50</v>
-      </c>
-      <c r="L9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>292</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>48</v>
-      </c>
-      <c r="K10">
-        <v>50</v>
-      </c>
-      <c r="L10">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>293</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>47</v>
-      </c>
-      <c r="K11">
-        <v>50</v>
-      </c>
-      <c r="L11">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>294</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>46</v>
-      </c>
-      <c r="K12">
-        <v>50</v>
-      </c>
-      <c r="L12">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>295</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>45</v>
-      </c>
-      <c r="K13">
-        <v>50</v>
-      </c>
-      <c r="L13">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>296</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>6</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>46</v>
-      </c>
-      <c r="K14">
-        <v>50</v>
-      </c>
-      <c r="L14">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>297</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>4</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>36</v>
-      </c>
-      <c r="K15">
-        <v>40</v>
-      </c>
-      <c r="L15">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>298</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <v>45</v>
-      </c>
-      <c r="K16">
-        <v>50</v>
-      </c>
-      <c r="L16">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>299</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>42</v>
-      </c>
-      <c r="K17">
-        <v>50</v>
-      </c>
-      <c r="L17">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>300</v>
-      </c>
-      <c r="B18">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>57</v>
-      </c>
-      <c r="K18">
-        <v>74</v>
-      </c>
-      <c r="L18">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>301</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>6</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>44</v>
-      </c>
-      <c r="K19">
-        <v>50</v>
-      </c>
-      <c r="L19">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>302</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>4</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>43</v>
-      </c>
-      <c r="K20">
-        <v>50</v>
-      </c>
-      <c r="L20">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>303</v>
-      </c>
-      <c r="B21">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>37</v>
-      </c>
-      <c r="K21">
-        <v>50</v>
-      </c>
-      <c r="L21">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>304</v>
-      </c>
-      <c r="B22">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>3</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>57</v>
-      </c>
-      <c r="K22">
-        <v>68</v>
-      </c>
-      <c r="L22">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>305</v>
-      </c>
-      <c r="B23">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>43</v>
-      </c>
-      <c r="K23">
-        <v>50</v>
-      </c>
-      <c r="L23">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>306</v>
-      </c>
-      <c r="B24">
-        <v>11</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>6</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>39</v>
-      </c>
-      <c r="K24">
-        <v>50</v>
-      </c>
-      <c r="L24">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>307</v>
-      </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>6</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>34</v>
-      </c>
-      <c r="K25">
-        <v>50</v>
-      </c>
-      <c r="L25">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>308</v>
-      </c>
-      <c r="B26">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>3</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>41</v>
-      </c>
-      <c r="K26">
-        <v>53</v>
-      </c>
-      <c r="L26">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>309</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>49</v>
-      </c>
-      <c r="K27">
-        <v>50</v>
-      </c>
-      <c r="L27">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>310</v>
-      </c>
-      <c r="B28">
-        <v>15</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>3</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>34</v>
-      </c>
-      <c r="K28">
-        <v>50</v>
-      </c>
-      <c r="L28">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>311</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>5</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>62</v>
-      </c>
-      <c r="K29">
-        <v>66</v>
-      </c>
-      <c r="L29">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>312</v>
-      </c>
-      <c r="B30">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>3</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>42</v>
-      </c>
-      <c r="K30">
-        <v>50</v>
-      </c>
-      <c r="L30">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>313</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>5</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>47</v>
-      </c>
-      <c r="K31">
-        <v>50</v>
-      </c>
-      <c r="L31">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>314</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>47</v>
-      </c>
-      <c r="K32">
-        <v>50</v>
-      </c>
-      <c r="L32">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>315</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>47</v>
-      </c>
-      <c r="K33">
-        <v>50</v>
-      </c>
-      <c r="L33">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>316</v>
-      </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>50</v>
-      </c>
-      <c r="K34">
-        <v>58</v>
-      </c>
-      <c r="L34">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>317</v>
-      </c>
-      <c r="B35">
-        <v>7</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>3</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>43</v>
-      </c>
-      <c r="K35">
-        <v>50</v>
-      </c>
-      <c r="L35">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>318</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>4</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>47</v>
-      </c>
-      <c r="K36">
-        <v>50</v>
-      </c>
-      <c r="L36">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>319</v>
-      </c>
-      <c r="B37">
-        <v>9</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>4</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>62</v>
-      </c>
-      <c r="K37">
-        <v>72</v>
-      </c>
-      <c r="L37">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>320</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>2</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>48</v>
-      </c>
-      <c r="K38">
-        <v>50</v>
-      </c>
-      <c r="L38">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>321</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>2</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>46</v>
-      </c>
-      <c r="K39">
-        <v>50</v>
-      </c>
-      <c r="L39">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>322</v>
-      </c>
-      <c r="B40">
-        <v>8</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>42</v>
-      </c>
-      <c r="K40">
-        <v>50</v>
-      </c>
-      <c r="L40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>323</v>
-      </c>
-      <c r="B41">
-        <v>7</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>43</v>
-      </c>
-      <c r="K41">
-        <v>50</v>
-      </c>
-      <c r="L41">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>324</v>
-      </c>
-      <c r="B42">
-        <v>7</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>25</v>
-      </c>
-      <c r="K42">
-        <v>32</v>
-      </c>
-      <c r="L42">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>325</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>47</v>
-      </c>
-      <c r="K43">
-        <v>50</v>
-      </c>
-      <c r="L43">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>326</v>
-      </c>
-      <c r="B44">
-        <v>10</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>40</v>
-      </c>
-      <c r="K44">
-        <v>50</v>
-      </c>
-      <c r="L44">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>327</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>46</v>
-      </c>
-      <c r="K45">
-        <v>50</v>
-      </c>
-      <c r="L45">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>328</v>
-      </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <v>47</v>
-      </c>
-      <c r="K46">
-        <v>50</v>
-      </c>
-      <c r="L46">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>329</v>
-      </c>
-      <c r="B47">
-        <v>9</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <v>40</v>
-      </c>
-      <c r="K47">
-        <v>50</v>
-      </c>
-      <c r="L47">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>330</v>
-      </c>
-      <c r="B48">
-        <v>9</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
-        <v>4</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <v>39</v>
-      </c>
-      <c r="K48">
-        <v>50</v>
-      </c>
-      <c r="L48">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>331</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-      <c r="J49">
-        <v>45</v>
-      </c>
-      <c r="K49">
-        <v>50</v>
-      </c>
-      <c r="L49">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>332</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="J50">
-        <v>24</v>
-      </c>
-      <c r="K50">
-        <v>28</v>
-      </c>
-      <c r="L50">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>333</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-      <c r="J51">
-        <v>19</v>
-      </c>
-      <c r="K51">
-        <v>23</v>
-      </c>
-      <c r="L51">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>334</v>
-      </c>
-      <c r="B52">
-        <v>2</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-      <c r="J52">
-        <v>16</v>
-      </c>
-      <c r="K52">
-        <v>19</v>
-      </c>
-      <c r="L52">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>335</v>
-      </c>
-      <c r="B53">
-        <v>5</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <v>12</v>
-      </c>
-      <c r="K53">
-        <v>18</v>
-      </c>
-      <c r="L53">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>336</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
-      </c>
-      <c r="J54">
-        <v>14</v>
-      </c>
-      <c r="K54">
-        <v>18</v>
-      </c>
-      <c r="L54">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>337</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55">
-        <v>17</v>
-      </c>
-      <c r="K55">
-        <v>18</v>
-      </c>
-      <c r="L55">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>338</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <v>13</v>
-      </c>
-      <c r="K56">
-        <v>18</v>
-      </c>
-      <c r="L56">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>339</v>
-      </c>
-      <c r="B57">
-        <v>2</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <v>15</v>
-      </c>
-      <c r="K57">
-        <v>18</v>
-      </c>
-      <c r="L57">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>340</v>
-      </c>
-      <c r="B58">
-        <v>2</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="J58">
-        <v>17</v>
-      </c>
-      <c r="K58">
-        <v>20</v>
-      </c>
-      <c r="L58">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>341</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>1</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-      <c r="J59">
-        <v>14</v>
-      </c>
-      <c r="K59">
-        <v>18</v>
-      </c>
-      <c r="L59">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>342</v>
-      </c>
-      <c r="B60">
-        <v>2</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>15</v>
-      </c>
-      <c r="K60">
-        <v>18</v>
-      </c>
-      <c r="L60">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>343</v>
-      </c>
-      <c r="B61">
-        <v>6</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-      <c r="J61">
-        <v>15</v>
-      </c>
-      <c r="K61">
-        <v>22</v>
-      </c>
-      <c r="L61">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>344</v>
-      </c>
-      <c r="B62">
-        <v>6</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <v>9</v>
-      </c>
-      <c r="K62">
-        <v>16</v>
-      </c>
-      <c r="L62">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>345</v>
-      </c>
-      <c r="B63">
-        <v>5</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <v>15</v>
-      </c>
-      <c r="K63">
-        <v>22</v>
-      </c>
-      <c r="L63">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="32">
-        <v>2.5833333333333335</v>
-      </c>
-      <c r="C64">
-        <v>354</v>
-      </c>
-      <c r="D64">
-        <v>3</v>
-      </c>
-      <c r="E64">
-        <v>15</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>28</v>
-      </c>
-      <c r="H64">
-        <v>133</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="J64">
-        <v>4</v>
-      </c>
-      <c r="K64" t="s">
-        <v>346</v>
+      <c r="J68" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F69" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J69">
+        <f>SUM(J65:J68)</f>
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>SUM(F65:F69)</f>
+        <v>502</v>
+      </c>
+      <c r="J70" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>112</v>
+      </c>
+      <c r="F71">
+        <f>K64-F70</f>
+        <v>2225</v>
+      </c>
+      <c r="J71">
+        <f>J69-L64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F72" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f>F71+F70</f>
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f>F73-K64</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15397,7 +15519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="132" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="102" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
@@ -15419,7 +15541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="115.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
nmv 20 07 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0CE85-DEF7-48A4-92C2-0F359A06192C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020E2EE-41B5-4CA4-B591-6BAB0EFC099A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="15" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="5.3" sheetId="17" r:id="rId3"/>
     <sheet name="5.4" sheetId="18" r:id="rId4"/>
     <sheet name="5.5" sheetId="19" r:id="rId5"/>
-    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId6"/>
+    <sheet name="5.6" sheetId="20" r:id="rId6"/>
+    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="402">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -2277,6 +2278,171 @@
   <si>
     <t>62</t>
   </si>
+  <si>
+    <t>5.6.1.1 :</t>
+  </si>
+  <si>
+    <t>5.6.1.2 :</t>
+  </si>
+  <si>
+    <t>5.6.1.3 :</t>
+  </si>
+  <si>
+    <t>5.6.1.4 :</t>
+  </si>
+  <si>
+    <t>5.6.2.1 :</t>
+  </si>
+  <si>
+    <t>5.6.2.2 :</t>
+  </si>
+  <si>
+    <t>5.6.2.3 :</t>
+  </si>
+  <si>
+    <t>5.6.2.4 :</t>
+  </si>
+  <si>
+    <t>5.6.2.5 :</t>
+  </si>
+  <si>
+    <t>5.6.2.6 :</t>
+  </si>
+  <si>
+    <t>5.6.3.1 :</t>
+  </si>
+  <si>
+    <t>5.6.3.2 :</t>
+  </si>
+  <si>
+    <t>5.6.3.3 :</t>
+  </si>
+  <si>
+    <t>5.6.3.4 :</t>
+  </si>
+  <si>
+    <t>5.6.4.1 :</t>
+  </si>
+  <si>
+    <t>5.6.4.2 :</t>
+  </si>
+  <si>
+    <t>5.6.4.3 :</t>
+  </si>
+  <si>
+    <t>5.6.4.4 :</t>
+  </si>
+  <si>
+    <t>5.6.4.5 :</t>
+  </si>
+  <si>
+    <t>5.6.5.1 :</t>
+  </si>
+  <si>
+    <t>5.6.5.2 :</t>
+  </si>
+  <si>
+    <t>5.6.5.3 :</t>
+  </si>
+  <si>
+    <t>5.6.6.1 :</t>
+  </si>
+  <si>
+    <t>5.6.6.2 :</t>
+  </si>
+  <si>
+    <t>5.6.6.3 :</t>
+  </si>
+  <si>
+    <t>5.6.6.4 :</t>
+  </si>
+  <si>
+    <t>5.6.7.1 :</t>
+  </si>
+  <si>
+    <t>5.6.7.2 :</t>
+  </si>
+  <si>
+    <t>5.6.7.3 :</t>
+  </si>
+  <si>
+    <t>5.6.8.1 :</t>
+  </si>
+  <si>
+    <t>5.6.8.2 :</t>
+  </si>
+  <si>
+    <t>5.6.8.3 :</t>
+  </si>
+  <si>
+    <t>5.6.8.4 :</t>
+  </si>
+  <si>
+    <t>5.6.8.5 :</t>
+  </si>
+  <si>
+    <t>5.6.8.6 :</t>
+  </si>
+  <si>
+    <t>5.6.9.1 :</t>
+  </si>
+  <si>
+    <t>5.6.9.2 :</t>
+  </si>
+  <si>
+    <t>5.6.9.3 :</t>
+  </si>
+  <si>
+    <t>5.6.10.1 :</t>
+  </si>
+  <si>
+    <t>5.6.10.2 :</t>
+  </si>
+  <si>
+    <t>5.6.10.3 :</t>
+  </si>
+  <si>
+    <t>5.6.11.1 :</t>
+  </si>
+  <si>
+    <t>5.6.12.1 :</t>
+  </si>
+  <si>
+    <t>5.6.13.1 :</t>
+  </si>
+  <si>
+    <t>5.6.14.1 :</t>
+  </si>
+  <si>
+    <t>5.6.15.1 :</t>
+  </si>
+  <si>
+    <t>5.6.16.1 :</t>
+  </si>
+  <si>
+    <t>5.6.17.1 :</t>
+  </si>
+  <si>
+    <t>5.6.18.1 :</t>
+  </si>
+  <si>
+    <t>5.6.19.1 :</t>
+  </si>
+  <si>
+    <t>5.6.20.1 :</t>
+  </si>
+  <si>
+    <t>5.6.21.1 :</t>
+  </si>
+  <si>
+    <t>5.6.22.1 :</t>
+  </si>
+  <si>
+    <t>5.6.23.1 :</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
 </sst>
 </file>
 
@@ -2472,7 +2638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2574,7 +2740,6 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12425,9 +12590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64BAEC-8D94-4B07-A1DD-3D546E3471DD}">
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65:K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14888,10 +15053,10 @@
       </c>
     </row>
     <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="39"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
       <c r="E65" t="s">
         <v>106</v>
       </c>
@@ -14903,8 +15068,8 @@
         <f>B64-C64</f>
         <v>350</v>
       </c>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
+      <c r="K65" s="34"/>
+      <c r="L65" s="34"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
@@ -14997,6 +15162,2272 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C046FF-F6CD-427B-B2BF-D07232B58F7D}">
+  <dimension ref="A1:L66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="33">
+        <v>5</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>1</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>5</v>
+      </c>
+      <c r="G2" s="33">
+        <v>0</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>39</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="33">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33">
+        <v>1</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>6</v>
+      </c>
+      <c r="G3" s="33">
+        <v>3</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>1</v>
+      </c>
+      <c r="J3" s="33">
+        <v>41</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="33">
+        <v>5</v>
+      </c>
+      <c r="C4" s="33">
+        <v>1</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>6</v>
+      </c>
+      <c r="G4" s="33">
+        <v>3</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>40</v>
+      </c>
+      <c r="K4" s="33">
+        <v>50</v>
+      </c>
+      <c r="L4" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="33">
+        <v>7</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>10</v>
+      </c>
+      <c r="G5" s="33">
+        <v>3</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>2</v>
+      </c>
+      <c r="J5" s="33">
+        <v>55</v>
+      </c>
+      <c r="K5" s="33">
+        <v>72</v>
+      </c>
+      <c r="L5" s="33">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="B6" s="33">
+        <v>8</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>2</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>41</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="B7" s="33">
+        <v>8</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>2</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>42</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="B8" s="33">
+        <v>6</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>4</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>43</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B9" s="33">
+        <v>5</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>2</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>45</v>
+      </c>
+      <c r="K9" s="33">
+        <v>50</v>
+      </c>
+      <c r="L9" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="33">
+        <v>9</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>2</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>41</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" s="33">
+        <v>4</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1</v>
+      </c>
+      <c r="G11" s="33">
+        <v>3</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>42</v>
+      </c>
+      <c r="K11" s="33">
+        <v>47</v>
+      </c>
+      <c r="L11" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" s="33">
+        <v>9</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>2</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>41</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="B13" s="33">
+        <v>9</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>6</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>41</v>
+      </c>
+      <c r="K13" s="33">
+        <v>50</v>
+      </c>
+      <c r="L13" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>5</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>46</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B15" s="33">
+        <v>5</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>42</v>
+      </c>
+      <c r="K15" s="33">
+        <v>48</v>
+      </c>
+      <c r="L15" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="B16" s="33">
+        <v>12</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>1</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>3</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>37</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="B17" s="33">
+        <v>4</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>1</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>2</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>45</v>
+      </c>
+      <c r="K17" s="33">
+        <v>50</v>
+      </c>
+      <c r="L17" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="B18" s="33">
+        <v>6</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>1</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>44</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="B19" s="33">
+        <v>4</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>4</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>46</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="B20" s="33">
+        <v>0</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>1</v>
+      </c>
+      <c r="G20" s="33">
+        <v>3</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>31</v>
+      </c>
+      <c r="K20" s="33">
+        <v>32</v>
+      </c>
+      <c r="L20" s="33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="B21" s="33">
+        <v>15</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>1</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>35</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>367</v>
+      </c>
+      <c r="B22" s="33">
+        <v>10</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>0</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>40</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" s="33">
+        <v>9</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>1</v>
+      </c>
+      <c r="G23" s="33">
+        <v>0</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>44</v>
+      </c>
+      <c r="K23" s="33">
+        <v>54</v>
+      </c>
+      <c r="L23" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>369</v>
+      </c>
+      <c r="B24" s="33">
+        <v>7</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>1</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
+        <v>5</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>42</v>
+      </c>
+      <c r="K24" s="33">
+        <v>50</v>
+      </c>
+      <c r="L24" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>370</v>
+      </c>
+      <c r="B25" s="33">
+        <v>8</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>2</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>5</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>40</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="B26" s="33">
+        <v>5</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>0</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>45</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="B27" s="33">
+        <v>2</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>1</v>
+      </c>
+      <c r="G27" s="33">
+        <v>5</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>57</v>
+      </c>
+      <c r="K27" s="33">
+        <v>60</v>
+      </c>
+      <c r="L27" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="B28" s="33">
+        <v>17</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>0</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>33</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>374</v>
+      </c>
+      <c r="B29" s="33">
+        <v>24</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>0</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>26</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>375</v>
+      </c>
+      <c r="B30" s="33">
+        <v>13</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>1</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1</v>
+      </c>
+      <c r="G30" s="33">
+        <v>3</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>63</v>
+      </c>
+      <c r="K30" s="33">
+        <v>78</v>
+      </c>
+      <c r="L30" s="33">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="B31" s="33">
+        <v>10</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <v>3</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>40</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="B32" s="33">
+        <v>9</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <v>4</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>41</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>378</v>
+      </c>
+      <c r="B33" s="33">
+        <v>7</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="33">
+        <v>2</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33">
+        <v>43</v>
+      </c>
+      <c r="K33" s="33">
+        <v>50</v>
+      </c>
+      <c r="L33" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="B34" s="33">
+        <v>5</v>
+      </c>
+      <c r="C34" s="33">
+        <v>0</v>
+      </c>
+      <c r="D34" s="33">
+        <v>2</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
+        <v>5</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>43</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="B35" s="33">
+        <v>6</v>
+      </c>
+      <c r="C35" s="33">
+        <v>0</v>
+      </c>
+      <c r="D35" s="33">
+        <v>1</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>0</v>
+      </c>
+      <c r="G35" s="33">
+        <v>2</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>43</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="B36" s="33">
+        <v>6</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>2</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>1</v>
+      </c>
+      <c r="G36" s="33">
+        <v>3</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>48</v>
+      </c>
+      <c r="K36" s="33">
+        <v>57</v>
+      </c>
+      <c r="L36" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="B37" s="33">
+        <v>6</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0</v>
+      </c>
+      <c r="D37" s="33">
+        <v>2</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>0</v>
+      </c>
+      <c r="G37" s="33">
+        <v>1</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>42</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>383</v>
+      </c>
+      <c r="B38" s="33">
+        <v>6</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>1</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>44</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="B39" s="33">
+        <v>9</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>1</v>
+      </c>
+      <c r="G39" s="33">
+        <v>3</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>60</v>
+      </c>
+      <c r="K39" s="33">
+        <v>70</v>
+      </c>
+      <c r="L39" s="33">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>385</v>
+      </c>
+      <c r="B40" s="33">
+        <v>9</v>
+      </c>
+      <c r="C40" s="33">
+        <v>0</v>
+      </c>
+      <c r="D40" s="33">
+        <v>1</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0</v>
+      </c>
+      <c r="G40" s="33">
+        <v>1</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>40</v>
+      </c>
+      <c r="K40" s="33">
+        <v>50</v>
+      </c>
+      <c r="L40" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>386</v>
+      </c>
+      <c r="B41" s="33">
+        <v>4</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>0</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>46</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="B42" s="33">
+        <v>13</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>1</v>
+      </c>
+      <c r="G42" s="33">
+        <v>5</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>49</v>
+      </c>
+      <c r="K42" s="33">
+        <v>65</v>
+      </c>
+      <c r="L42" s="33">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="B43" s="33">
+        <v>10</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>1</v>
+      </c>
+      <c r="G43" s="33">
+        <v>0</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>15</v>
+      </c>
+      <c r="K43" s="33">
+        <v>26</v>
+      </c>
+      <c r="L43" s="33">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>389</v>
+      </c>
+      <c r="B44" s="33">
+        <v>8</v>
+      </c>
+      <c r="C44" s="33">
+        <v>0</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>1</v>
+      </c>
+      <c r="G44" s="33">
+        <v>0</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>17</v>
+      </c>
+      <c r="K44" s="33">
+        <v>26</v>
+      </c>
+      <c r="L44" s="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>390</v>
+      </c>
+      <c r="B45" s="33">
+        <v>14</v>
+      </c>
+      <c r="C45" s="33">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>1</v>
+      </c>
+      <c r="G45" s="33">
+        <v>0</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>10</v>
+      </c>
+      <c r="K45" s="33">
+        <v>25</v>
+      </c>
+      <c r="L45" s="33">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="B46" s="33">
+        <v>14</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>1</v>
+      </c>
+      <c r="G46" s="33">
+        <v>0</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>10</v>
+      </c>
+      <c r="K46" s="33">
+        <v>25</v>
+      </c>
+      <c r="L46" s="33">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="B47" s="33">
+        <v>3</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>1</v>
+      </c>
+      <c r="G47" s="33">
+        <v>0</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>19</v>
+      </c>
+      <c r="K47" s="33">
+        <v>23</v>
+      </c>
+      <c r="L47" s="33">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>393</v>
+      </c>
+      <c r="B48" s="33">
+        <v>7</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>0</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>1</v>
+      </c>
+      <c r="G48" s="33">
+        <v>0</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>12</v>
+      </c>
+      <c r="K48" s="33">
+        <v>20</v>
+      </c>
+      <c r="L48" s="33">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="B49" s="33">
+        <v>6</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>1</v>
+      </c>
+      <c r="G49" s="33">
+        <v>0</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>15</v>
+      </c>
+      <c r="K49" s="33">
+        <v>22</v>
+      </c>
+      <c r="L49" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="B50" s="33">
+        <v>5</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>0</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>1</v>
+      </c>
+      <c r="G50" s="33">
+        <v>0</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>12</v>
+      </c>
+      <c r="K50" s="33">
+        <v>18</v>
+      </c>
+      <c r="L50" s="33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="B51" s="33">
+        <v>2</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>1</v>
+      </c>
+      <c r="G51" s="33">
+        <v>0</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>16</v>
+      </c>
+      <c r="K51" s="33">
+        <v>19</v>
+      </c>
+      <c r="L51" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>397</v>
+      </c>
+      <c r="B52" s="33">
+        <v>8</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>0</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>1</v>
+      </c>
+      <c r="G52" s="33">
+        <v>0</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>11</v>
+      </c>
+      <c r="K52" s="33">
+        <v>20</v>
+      </c>
+      <c r="L52" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="B53" s="33">
+        <v>10</v>
+      </c>
+      <c r="C53" s="33">
+        <v>1</v>
+      </c>
+      <c r="D53" s="33">
+        <v>16</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>1</v>
+      </c>
+      <c r="G53" s="33">
+        <v>0</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>8</v>
+      </c>
+      <c r="K53" s="33">
+        <v>34</v>
+      </c>
+      <c r="L53" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="B54" s="33">
+        <v>3</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>0</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>1</v>
+      </c>
+      <c r="G54" s="33">
+        <v>2</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>21</v>
+      </c>
+      <c r="K54" s="33">
+        <v>25</v>
+      </c>
+      <c r="L54" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="B55" s="33">
+        <v>4</v>
+      </c>
+      <c r="C55" s="33">
+        <v>1</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>1</v>
+      </c>
+      <c r="G55" s="33">
+        <v>0</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>0</v>
+      </c>
+      <c r="J55" s="33">
+        <v>16</v>
+      </c>
+      <c r="K55" s="33">
+        <v>20</v>
+      </c>
+      <c r="L55" s="33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="37" t="s">
+        <v>401</v>
+      </c>
+      <c r="B56" s="37">
+        <f>SUM(B2:B55)</f>
+        <v>408</v>
+      </c>
+      <c r="C56" s="37">
+        <f t="shared" ref="C56:L56" si="0">SUM(C2:C55)</f>
+        <v>4</v>
+      </c>
+      <c r="D56" s="37">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E56" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="37">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="G56" s="37">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="H56" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="37">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J56" s="37">
+        <f t="shared" si="0"/>
+        <v>1948</v>
+      </c>
+      <c r="K56" s="37">
+        <f t="shared" si="0"/>
+        <v>2436</v>
+      </c>
+      <c r="L56" s="37">
+        <f t="shared" si="0"/>
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="32"/>
+      <c r="E57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F57">
+        <f>G56</f>
+        <v>104</v>
+      </c>
+      <c r="J57">
+        <f>B56-C56</f>
+        <v>404</v>
+      </c>
+      <c r="K57" s="34"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58">
+        <f>B56</f>
+        <v>408</v>
+      </c>
+      <c r="J58">
+        <f>D56-E56</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>108</v>
+      </c>
+      <c r="F59">
+        <v>33</v>
+      </c>
+      <c r="J59">
+        <f>F65</f>
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>109</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="J60" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F61" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J57:J60)</f>
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f>SUM(F57:F61)</f>
+        <v>547</v>
+      </c>
+      <c r="J62" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>112</v>
+      </c>
+      <c r="F63">
+        <f>K56-F62</f>
+        <v>1889</v>
+      </c>
+      <c r="J63">
+        <f>J61-L56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F64" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f>F63+F62</f>
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f>F65-K56</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 12 08 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 5.1 TO 5.7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020E2EE-41B5-4CA4-B591-6BAB0EFC099A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D67B31-A93F-4B03-9899-BD1F13A42DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1" sheetId="15" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="5.4" sheetId="18" r:id="rId4"/>
     <sheet name="5.5" sheetId="19" r:id="rId5"/>
     <sheet name="5.6" sheetId="20" r:id="rId6"/>
-    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId7"/>
+    <sheet name="5.7" sheetId="21" r:id="rId7"/>
+    <sheet name="total 5.1 to 5.7" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="460">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -2442,6 +2443,180 @@
   </si>
   <si>
     <t>54</t>
+  </si>
+  <si>
+    <t>5.7.1.1 :</t>
+  </si>
+  <si>
+    <t>5.7.1.2 :</t>
+  </si>
+  <si>
+    <t>5.7.1.3 :</t>
+  </si>
+  <si>
+    <t>5.7.2.1 :</t>
+  </si>
+  <si>
+    <t>5.7.2.2 :</t>
+  </si>
+  <si>
+    <t>5.7.2.3 :</t>
+  </si>
+  <si>
+    <t>5.7.2.4 :</t>
+  </si>
+  <si>
+    <t>5.7.2.5 :</t>
+  </si>
+  <si>
+    <t>5.7.3.1 :</t>
+  </si>
+  <si>
+    <t>5.7.3.2 :</t>
+  </si>
+  <si>
+    <t>5.7.3.3 :</t>
+  </si>
+  <si>
+    <t>5.7.3.4 :</t>
+  </si>
+  <si>
+    <t>5.7.4.1 :</t>
+  </si>
+  <si>
+    <t>5.7.4.2 :</t>
+  </si>
+  <si>
+    <t>5.7.4.3 :</t>
+  </si>
+  <si>
+    <t>5.7.4.4 :</t>
+  </si>
+  <si>
+    <t>5.7.5.1 :</t>
+  </si>
+  <si>
+    <t>5.7.5.2 :</t>
+  </si>
+  <si>
+    <t>5.7.5.3 :</t>
+  </si>
+  <si>
+    <t>5.7.5.4 :</t>
+  </si>
+  <si>
+    <t>5.7.5.5 :</t>
+  </si>
+  <si>
+    <t>5.7.5.6 :</t>
+  </si>
+  <si>
+    <t>5.7.5.7 :</t>
+  </si>
+  <si>
+    <t>5.7.6.1 :</t>
+  </si>
+  <si>
+    <t>5.7.6.2 :</t>
+  </si>
+  <si>
+    <t>5.7.6.3 :</t>
+  </si>
+  <si>
+    <t>5.7.6.4 :</t>
+  </si>
+  <si>
+    <t>5.7.6.5 :</t>
+  </si>
+  <si>
+    <t>5.7.6.6 :</t>
+  </si>
+  <si>
+    <t>5.7.7.1 :</t>
+  </si>
+  <si>
+    <t>5.7.7.2 :</t>
+  </si>
+  <si>
+    <t>5.7.7.3 :</t>
+  </si>
+  <si>
+    <t>5.7.8.1 :</t>
+  </si>
+  <si>
+    <t>5.7.8.2 :</t>
+  </si>
+  <si>
+    <t>5.7.8.3 :</t>
+  </si>
+  <si>
+    <t>5.7.9.1 :</t>
+  </si>
+  <si>
+    <t>5.7.9.2 :</t>
+  </si>
+  <si>
+    <t>5.7.9.3 :</t>
+  </si>
+  <si>
+    <t>5.7.9.4 :</t>
+  </si>
+  <si>
+    <t>5.7.10.1 :</t>
+  </si>
+  <si>
+    <t>5.7.10.2 :</t>
+  </si>
+  <si>
+    <t>5.7.10.3 :</t>
+  </si>
+  <si>
+    <t>5.7.11.1 :</t>
+  </si>
+  <si>
+    <t>5.7.12.1 :</t>
+  </si>
+  <si>
+    <t>5.7.13.1 :</t>
+  </si>
+  <si>
+    <t>5.7.14.1 :</t>
+  </si>
+  <si>
+    <t>5.7.15.1 :</t>
+  </si>
+  <si>
+    <t>5.7.16.1 :</t>
+  </si>
+  <si>
+    <t>5.7.17.1 :</t>
+  </si>
+  <si>
+    <t>5.7.18.1 :</t>
+  </si>
+  <si>
+    <t>5.7.19.1 :</t>
+  </si>
+  <si>
+    <t>5.7.20.1 :</t>
+  </si>
+  <si>
+    <t>5.7.21.1 :</t>
+  </si>
+  <si>
+    <t>5.7.22.1 :</t>
+  </si>
+  <si>
+    <t>5.7.23.1 :</t>
+  </si>
+  <si>
+    <t>5.7.24.1 :</t>
+  </si>
+  <si>
+    <t>5.7.25.1 :</t>
+  </si>
+  <si>
+    <t>5.7.26.1 :</t>
   </si>
 </sst>
 </file>
@@ -15165,9 +15340,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C046FF-F6CD-427B-B2BF-D07232B58F7D}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57:J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17428,11 +17603,2428 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA295860-D556-489E-AF88-BD8B70DE9F3B}">
+  <dimension ref="A1:L70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="B2" s="33">
+        <v>6</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
+        <v>4</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>44</v>
+      </c>
+      <c r="K2" s="33">
+        <v>50</v>
+      </c>
+      <c r="L2" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="B3" s="33">
+        <v>9</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
+        <v>3</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>41</v>
+      </c>
+      <c r="K3" s="33">
+        <v>50</v>
+      </c>
+      <c r="L3" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="B4" s="33">
+        <v>8</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>1</v>
+      </c>
+      <c r="G4" s="33">
+        <v>3</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>39</v>
+      </c>
+      <c r="K4" s="33">
+        <v>48</v>
+      </c>
+      <c r="L4" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>405</v>
+      </c>
+      <c r="B5" s="33">
+        <v>11</v>
+      </c>
+      <c r="C5" s="33">
+        <v>2</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>5</v>
+      </c>
+      <c r="G5" s="33">
+        <v>3</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>36</v>
+      </c>
+      <c r="K5" s="33">
+        <v>50</v>
+      </c>
+      <c r="L5" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>406</v>
+      </c>
+      <c r="B6" s="33">
+        <v>6</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>2</v>
+      </c>
+      <c r="G6" s="33">
+        <v>2</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>42</v>
+      </c>
+      <c r="K6" s="33">
+        <v>50</v>
+      </c>
+      <c r="L6" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="B7" s="33">
+        <v>11</v>
+      </c>
+      <c r="C7" s="33">
+        <v>2</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>3</v>
+      </c>
+      <c r="G7" s="33">
+        <v>3</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>37</v>
+      </c>
+      <c r="K7" s="33">
+        <v>50</v>
+      </c>
+      <c r="L7" s="33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" s="33">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>6</v>
+      </c>
+      <c r="G8" s="33">
+        <v>3</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33">
+        <v>1</v>
+      </c>
+      <c r="J8" s="33">
+        <v>36</v>
+      </c>
+      <c r="K8" s="33">
+        <v>50</v>
+      </c>
+      <c r="L8" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="33">
+        <v>15</v>
+      </c>
+      <c r="C9" s="33">
+        <v>1</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>2</v>
+      </c>
+      <c r="G9" s="33">
+        <v>5</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>59</v>
+      </c>
+      <c r="K9" s="33">
+        <v>75</v>
+      </c>
+      <c r="L9" s="33">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" s="33">
+        <v>10</v>
+      </c>
+      <c r="C10" s="33">
+        <v>1</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>2</v>
+      </c>
+      <c r="G10" s="33">
+        <v>4</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <v>39</v>
+      </c>
+      <c r="K10" s="33">
+        <v>50</v>
+      </c>
+      <c r="L10" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="B11" s="33">
+        <v>7</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>2</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>2</v>
+      </c>
+      <c r="G11" s="33">
+        <v>3</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="33">
+        <v>39</v>
+      </c>
+      <c r="K11" s="33">
+        <v>50</v>
+      </c>
+      <c r="L11" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12" s="33">
+        <v>4</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>1</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>1</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
+        <v>45</v>
+      </c>
+      <c r="K12" s="33">
+        <v>50</v>
+      </c>
+      <c r="L12" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="B13" s="33">
+        <v>3</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
+      <c r="G13" s="33">
+        <v>3</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
+        <v>42</v>
+      </c>
+      <c r="K13" s="33">
+        <v>46</v>
+      </c>
+      <c r="L13" s="33">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>414</v>
+      </c>
+      <c r="B14" s="33">
+        <v>6</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>1</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>4</v>
+      </c>
+      <c r="H14" s="33">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>43</v>
+      </c>
+      <c r="K14" s="33">
+        <v>50</v>
+      </c>
+      <c r="L14" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="B15" s="33">
+        <v>5</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>2</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>45</v>
+      </c>
+      <c r="K15" s="33">
+        <v>50</v>
+      </c>
+      <c r="L15" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="B16" s="33">
+        <v>7</v>
+      </c>
+      <c r="C16" s="33">
+        <v>1</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>4</v>
+      </c>
+      <c r="G16" s="33">
+        <v>4</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>40</v>
+      </c>
+      <c r="K16" s="33">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>417</v>
+      </c>
+      <c r="B17" s="33">
+        <v>9</v>
+      </c>
+      <c r="C17" s="33">
+        <v>1</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>5</v>
+      </c>
+      <c r="G17" s="33">
+        <v>8</v>
+      </c>
+      <c r="H17" s="33">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>44</v>
+      </c>
+      <c r="K17" s="33">
+        <v>57</v>
+      </c>
+      <c r="L17" s="33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>418</v>
+      </c>
+      <c r="B18" s="33">
+        <v>4</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>1</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0</v>
+      </c>
+      <c r="J18" s="33">
+        <v>46</v>
+      </c>
+      <c r="K18" s="33">
+        <v>50</v>
+      </c>
+      <c r="L18" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B19" s="33">
+        <v>0</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>1</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33">
+        <v>0</v>
+      </c>
+      <c r="J19" s="33">
+        <v>49</v>
+      </c>
+      <c r="K19" s="33">
+        <v>50</v>
+      </c>
+      <c r="L19" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>420</v>
+      </c>
+      <c r="B20" s="33">
+        <v>6</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="33">
+        <v>4</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33">
+        <v>0</v>
+      </c>
+      <c r="J20" s="33">
+        <v>44</v>
+      </c>
+      <c r="K20" s="33">
+        <v>50</v>
+      </c>
+      <c r="L20" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="B21" s="33">
+        <v>4</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <v>6</v>
+      </c>
+      <c r="H21" s="33">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <v>0</v>
+      </c>
+      <c r="J21" s="33">
+        <v>46</v>
+      </c>
+      <c r="K21" s="33">
+        <v>50</v>
+      </c>
+      <c r="L21" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>422</v>
+      </c>
+      <c r="B22" s="33">
+        <v>3</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0</v>
+      </c>
+      <c r="G22" s="33">
+        <v>6</v>
+      </c>
+      <c r="H22" s="33">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33">
+        <v>0</v>
+      </c>
+      <c r="J22" s="33">
+        <v>47</v>
+      </c>
+      <c r="K22" s="33">
+        <v>50</v>
+      </c>
+      <c r="L22" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="B23" s="33">
+        <v>8</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <v>5</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33">
+        <v>42</v>
+      </c>
+      <c r="K23" s="33">
+        <v>50</v>
+      </c>
+      <c r="L23" s="33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>424</v>
+      </c>
+      <c r="B24" s="33">
+        <v>4</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>1</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="33">
+        <v>1</v>
+      </c>
+      <c r="G24" s="33">
+        <v>4</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
+        <v>0</v>
+      </c>
+      <c r="J24" s="33">
+        <v>39</v>
+      </c>
+      <c r="K24" s="33">
+        <v>45</v>
+      </c>
+      <c r="L24" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>425</v>
+      </c>
+      <c r="B25" s="33">
+        <v>5</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0</v>
+      </c>
+      <c r="G25" s="33">
+        <v>2</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
+        <v>45</v>
+      </c>
+      <c r="K25" s="33">
+        <v>50</v>
+      </c>
+      <c r="L25" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>426</v>
+      </c>
+      <c r="B26" s="33">
+        <v>9</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="33">
+        <v>1</v>
+      </c>
+      <c r="H26" s="33">
+        <v>0</v>
+      </c>
+      <c r="I26" s="33">
+        <v>0</v>
+      </c>
+      <c r="J26" s="33">
+        <v>41</v>
+      </c>
+      <c r="K26" s="33">
+        <v>50</v>
+      </c>
+      <c r="L26" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="B27" s="33">
+        <v>5</v>
+      </c>
+      <c r="C27" s="33">
+        <v>1</v>
+      </c>
+      <c r="D27" s="33">
+        <v>2</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <v>4</v>
+      </c>
+      <c r="G27" s="33">
+        <v>1</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+      <c r="I27" s="33">
+        <v>0</v>
+      </c>
+      <c r="J27" s="33">
+        <v>40</v>
+      </c>
+      <c r="K27" s="33">
+        <v>50</v>
+      </c>
+      <c r="L27" s="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="B28" s="33">
+        <v>4</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>2</v>
+      </c>
+      <c r="G28" s="33">
+        <v>0</v>
+      </c>
+      <c r="H28" s="33">
+        <v>0</v>
+      </c>
+      <c r="I28" s="33">
+        <v>0</v>
+      </c>
+      <c r="J28" s="33">
+        <v>44</v>
+      </c>
+      <c r="K28" s="33">
+        <v>50</v>
+      </c>
+      <c r="L28" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>429</v>
+      </c>
+      <c r="B29" s="33">
+        <v>7</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <v>2</v>
+      </c>
+      <c r="H29" s="33">
+        <v>0</v>
+      </c>
+      <c r="I29" s="33">
+        <v>0</v>
+      </c>
+      <c r="J29" s="33">
+        <v>43</v>
+      </c>
+      <c r="K29" s="33">
+        <v>50</v>
+      </c>
+      <c r="L29" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="B30" s="33">
+        <v>9</v>
+      </c>
+      <c r="C30" s="33">
+        <v>0</v>
+      </c>
+      <c r="D30" s="33">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1</v>
+      </c>
+      <c r="G30" s="33">
+        <v>2</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="33">
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <v>43</v>
+      </c>
+      <c r="K30" s="33">
+        <v>53</v>
+      </c>
+      <c r="L30" s="33">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="B31" s="33">
+        <v>15</v>
+      </c>
+      <c r="C31" s="33">
+        <v>2</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <v>5</v>
+      </c>
+      <c r="G31" s="33">
+        <v>3</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33">
+        <v>0</v>
+      </c>
+      <c r="J31" s="33">
+        <v>32</v>
+      </c>
+      <c r="K31" s="33">
+        <v>50</v>
+      </c>
+      <c r="L31" s="33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>432</v>
+      </c>
+      <c r="B32" s="33">
+        <v>8</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="33">
+        <v>1</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <v>6</v>
+      </c>
+      <c r="G32" s="33">
+        <v>6</v>
+      </c>
+      <c r="H32" s="33">
+        <v>0</v>
+      </c>
+      <c r="I32" s="33">
+        <v>0</v>
+      </c>
+      <c r="J32" s="33">
+        <v>35</v>
+      </c>
+      <c r="K32" s="33">
+        <v>50</v>
+      </c>
+      <c r="L32" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="B33" s="33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
+        <v>9</v>
+      </c>
+      <c r="G33" s="33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="33">
+        <v>51</v>
+      </c>
+      <c r="K33" s="33">
+        <v>64</v>
+      </c>
+      <c r="L33" s="33">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="B34" s="33">
+        <v>6</v>
+      </c>
+      <c r="C34" s="33">
+        <v>1</v>
+      </c>
+      <c r="D34" s="33">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33">
+        <v>0</v>
+      </c>
+      <c r="F34" s="33">
+        <v>2</v>
+      </c>
+      <c r="G34" s="33">
+        <v>0</v>
+      </c>
+      <c r="H34" s="33">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>43</v>
+      </c>
+      <c r="K34" s="33">
+        <v>50</v>
+      </c>
+      <c r="L34" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B35" s="33">
+        <v>6</v>
+      </c>
+      <c r="C35" s="33">
+        <v>2</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33">
+        <v>2</v>
+      </c>
+      <c r="G35" s="33">
+        <v>3</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33">
+        <v>0</v>
+      </c>
+      <c r="J35" s="33">
+        <v>44</v>
+      </c>
+      <c r="K35" s="33">
+        <v>50</v>
+      </c>
+      <c r="L35" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="B36" s="33">
+        <v>16</v>
+      </c>
+      <c r="C36" s="33">
+        <v>0</v>
+      </c>
+      <c r="D36" s="33">
+        <v>1</v>
+      </c>
+      <c r="E36" s="33">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33">
+        <v>1</v>
+      </c>
+      <c r="G36" s="33">
+        <v>2</v>
+      </c>
+      <c r="H36" s="33">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33">
+        <v>0</v>
+      </c>
+      <c r="J36" s="33">
+        <v>48</v>
+      </c>
+      <c r="K36" s="33">
+        <v>66</v>
+      </c>
+      <c r="L36" s="33">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="B37" s="33">
+        <v>7</v>
+      </c>
+      <c r="C37" s="33">
+        <v>3</v>
+      </c>
+      <c r="D37" s="33">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+      <c r="F37" s="33">
+        <v>4</v>
+      </c>
+      <c r="G37" s="33">
+        <v>3</v>
+      </c>
+      <c r="H37" s="33">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33">
+        <v>0</v>
+      </c>
+      <c r="J37" s="33">
+        <v>42</v>
+      </c>
+      <c r="K37" s="33">
+        <v>50</v>
+      </c>
+      <c r="L37" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="B38" s="33">
+        <v>5</v>
+      </c>
+      <c r="C38" s="33">
+        <v>0</v>
+      </c>
+      <c r="D38" s="33">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33">
+        <v>0</v>
+      </c>
+      <c r="F38" s="33">
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <v>3</v>
+      </c>
+      <c r="H38" s="33">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33">
+        <v>0</v>
+      </c>
+      <c r="J38" s="33">
+        <v>45</v>
+      </c>
+      <c r="K38" s="33">
+        <v>50</v>
+      </c>
+      <c r="L38" s="33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>439</v>
+      </c>
+      <c r="B39" s="33">
+        <v>3</v>
+      </c>
+      <c r="C39" s="33">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33">
+        <v>1</v>
+      </c>
+      <c r="E39" s="33">
+        <v>0</v>
+      </c>
+      <c r="F39" s="33">
+        <v>0</v>
+      </c>
+      <c r="G39" s="33">
+        <v>1</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+      <c r="I39" s="33">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>46</v>
+      </c>
+      <c r="K39" s="33">
+        <v>50</v>
+      </c>
+      <c r="L39" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="B40" s="33">
+        <v>8</v>
+      </c>
+      <c r="C40" s="33">
+        <v>1</v>
+      </c>
+      <c r="D40" s="33">
+        <v>2</v>
+      </c>
+      <c r="E40" s="33">
+        <v>0</v>
+      </c>
+      <c r="F40" s="33">
+        <v>1</v>
+      </c>
+      <c r="G40" s="33">
+        <v>5</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33">
+        <v>0</v>
+      </c>
+      <c r="J40" s="33">
+        <v>65</v>
+      </c>
+      <c r="K40" s="33">
+        <v>75</v>
+      </c>
+      <c r="L40" s="33">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>441</v>
+      </c>
+      <c r="B41" s="33">
+        <v>3</v>
+      </c>
+      <c r="C41" s="33">
+        <v>0</v>
+      </c>
+      <c r="D41" s="33">
+        <v>0</v>
+      </c>
+      <c r="E41" s="33">
+        <v>0</v>
+      </c>
+      <c r="F41" s="33">
+        <v>0</v>
+      </c>
+      <c r="G41" s="33">
+        <v>9</v>
+      </c>
+      <c r="H41" s="33">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33">
+        <v>0</v>
+      </c>
+      <c r="J41" s="33">
+        <v>47</v>
+      </c>
+      <c r="K41" s="33">
+        <v>50</v>
+      </c>
+      <c r="L41" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>442</v>
+      </c>
+      <c r="B42" s="33">
+        <v>8</v>
+      </c>
+      <c r="C42" s="33">
+        <v>0</v>
+      </c>
+      <c r="D42" s="33">
+        <v>1</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>3</v>
+      </c>
+      <c r="H42" s="33">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33">
+        <v>0</v>
+      </c>
+      <c r="J42" s="33">
+        <v>41</v>
+      </c>
+      <c r="K42" s="33">
+        <v>50</v>
+      </c>
+      <c r="L42" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="B43" s="33">
+        <v>3</v>
+      </c>
+      <c r="C43" s="33">
+        <v>0</v>
+      </c>
+      <c r="D43" s="33">
+        <v>0</v>
+      </c>
+      <c r="E43" s="33">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <v>1</v>
+      </c>
+      <c r="G43" s="33">
+        <v>4</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33">
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <v>46</v>
+      </c>
+      <c r="K43" s="33">
+        <v>50</v>
+      </c>
+      <c r="L43" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>444</v>
+      </c>
+      <c r="B44" s="33">
+        <v>4</v>
+      </c>
+      <c r="C44" s="33">
+        <v>1</v>
+      </c>
+      <c r="D44" s="33">
+        <v>0</v>
+      </c>
+      <c r="E44" s="33">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <v>1</v>
+      </c>
+      <c r="G44" s="33">
+        <v>0</v>
+      </c>
+      <c r="H44" s="33">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33">
+        <v>0</v>
+      </c>
+      <c r="J44" s="33">
+        <v>18</v>
+      </c>
+      <c r="K44" s="33">
+        <v>22</v>
+      </c>
+      <c r="L44" s="33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>445</v>
+      </c>
+      <c r="B45" s="33">
+        <v>10</v>
+      </c>
+      <c r="C45" s="33">
+        <v>1</v>
+      </c>
+      <c r="D45" s="33">
+        <v>1</v>
+      </c>
+      <c r="E45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <v>1</v>
+      </c>
+      <c r="G45" s="33">
+        <v>0</v>
+      </c>
+      <c r="H45" s="33">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33">
+        <v>0</v>
+      </c>
+      <c r="J45" s="33">
+        <v>14</v>
+      </c>
+      <c r="K45" s="33">
+        <v>25</v>
+      </c>
+      <c r="L45" s="33">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>446</v>
+      </c>
+      <c r="B46" s="33">
+        <v>5</v>
+      </c>
+      <c r="C46" s="33">
+        <v>0</v>
+      </c>
+      <c r="D46" s="33">
+        <v>0</v>
+      </c>
+      <c r="E46" s="33">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <v>1</v>
+      </c>
+      <c r="G46" s="33">
+        <v>0</v>
+      </c>
+      <c r="H46" s="33">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33">
+        <v>0</v>
+      </c>
+      <c r="J46" s="33">
+        <v>17</v>
+      </c>
+      <c r="K46" s="33">
+        <v>23</v>
+      </c>
+      <c r="L46" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="B47" s="33">
+        <v>7</v>
+      </c>
+      <c r="C47" s="33">
+        <v>0</v>
+      </c>
+      <c r="D47" s="33">
+        <v>0</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <v>1</v>
+      </c>
+      <c r="G47" s="33">
+        <v>0</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33">
+        <v>0</v>
+      </c>
+      <c r="J47" s="33">
+        <v>13</v>
+      </c>
+      <c r="K47" s="33">
+        <v>21</v>
+      </c>
+      <c r="L47" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>448</v>
+      </c>
+      <c r="B48" s="33">
+        <v>6</v>
+      </c>
+      <c r="C48" s="33">
+        <v>0</v>
+      </c>
+      <c r="D48" s="33">
+        <v>3</v>
+      </c>
+      <c r="E48" s="33">
+        <v>0</v>
+      </c>
+      <c r="F48" s="33">
+        <v>1</v>
+      </c>
+      <c r="G48" s="33">
+        <v>0</v>
+      </c>
+      <c r="H48" s="33">
+        <v>0</v>
+      </c>
+      <c r="I48" s="33">
+        <v>0</v>
+      </c>
+      <c r="J48" s="33">
+        <v>12</v>
+      </c>
+      <c r="K48" s="33">
+        <v>22</v>
+      </c>
+      <c r="L48" s="33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>449</v>
+      </c>
+      <c r="B49" s="33">
+        <v>2</v>
+      </c>
+      <c r="C49" s="33">
+        <v>0</v>
+      </c>
+      <c r="D49" s="33">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33">
+        <v>1</v>
+      </c>
+      <c r="G49" s="33">
+        <v>0</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="33">
+        <v>0</v>
+      </c>
+      <c r="J49" s="33">
+        <v>19</v>
+      </c>
+      <c r="K49" s="33">
+        <v>22</v>
+      </c>
+      <c r="L49" s="33">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>450</v>
+      </c>
+      <c r="B50" s="33">
+        <v>3</v>
+      </c>
+      <c r="C50" s="33">
+        <v>0</v>
+      </c>
+      <c r="D50" s="33">
+        <v>0</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+      <c r="F50" s="33">
+        <v>1</v>
+      </c>
+      <c r="G50" s="33">
+        <v>0</v>
+      </c>
+      <c r="H50" s="33">
+        <v>0</v>
+      </c>
+      <c r="I50" s="33">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33">
+        <v>20</v>
+      </c>
+      <c r="K50" s="33">
+        <v>24</v>
+      </c>
+      <c r="L50" s="33">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>451</v>
+      </c>
+      <c r="B51" s="33">
+        <v>7</v>
+      </c>
+      <c r="C51" s="33">
+        <v>0</v>
+      </c>
+      <c r="D51" s="33">
+        <v>0</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+      <c r="F51" s="33">
+        <v>1</v>
+      </c>
+      <c r="G51" s="33">
+        <v>0</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+      <c r="I51" s="33">
+        <v>0</v>
+      </c>
+      <c r="J51" s="33">
+        <v>12</v>
+      </c>
+      <c r="K51" s="33">
+        <v>20</v>
+      </c>
+      <c r="L51" s="33">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>452</v>
+      </c>
+      <c r="B52" s="33">
+        <v>9</v>
+      </c>
+      <c r="C52" s="33">
+        <v>0</v>
+      </c>
+      <c r="D52" s="33">
+        <v>0</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+      <c r="F52" s="33">
+        <v>1</v>
+      </c>
+      <c r="G52" s="33">
+        <v>0</v>
+      </c>
+      <c r="H52" s="33">
+        <v>0</v>
+      </c>
+      <c r="I52" s="33">
+        <v>0</v>
+      </c>
+      <c r="J52" s="33">
+        <v>6</v>
+      </c>
+      <c r="K52" s="33">
+        <v>16</v>
+      </c>
+      <c r="L52" s="33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="B53" s="33">
+        <v>4</v>
+      </c>
+      <c r="C53" s="33">
+        <v>0</v>
+      </c>
+      <c r="D53" s="33">
+        <v>0</v>
+      </c>
+      <c r="E53" s="33">
+        <v>0</v>
+      </c>
+      <c r="F53" s="33">
+        <v>1</v>
+      </c>
+      <c r="G53" s="33">
+        <v>0</v>
+      </c>
+      <c r="H53" s="33">
+        <v>0</v>
+      </c>
+      <c r="I53" s="33">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33">
+        <v>23</v>
+      </c>
+      <c r="K53" s="33">
+        <v>28</v>
+      </c>
+      <c r="L53" s="33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>454</v>
+      </c>
+      <c r="B54" s="33">
+        <v>3</v>
+      </c>
+      <c r="C54" s="33">
+        <v>0</v>
+      </c>
+      <c r="D54" s="33">
+        <v>0</v>
+      </c>
+      <c r="E54" s="33">
+        <v>0</v>
+      </c>
+      <c r="F54" s="33">
+        <v>1</v>
+      </c>
+      <c r="G54" s="33">
+        <v>0</v>
+      </c>
+      <c r="H54" s="33">
+        <v>0</v>
+      </c>
+      <c r="I54" s="33">
+        <v>0</v>
+      </c>
+      <c r="J54" s="33">
+        <v>25</v>
+      </c>
+      <c r="K54" s="33">
+        <v>29</v>
+      </c>
+      <c r="L54" s="33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>455</v>
+      </c>
+      <c r="B55" s="33">
+        <v>2</v>
+      </c>
+      <c r="C55" s="33">
+        <v>0</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33">
+        <v>0</v>
+      </c>
+      <c r="F55" s="33">
+        <v>1</v>
+      </c>
+      <c r="G55" s="33">
+        <v>0</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+      <c r="I55" s="33">
+        <v>0</v>
+      </c>
+      <c r="J55" s="33">
+        <v>25</v>
+      </c>
+      <c r="K55" s="33">
+        <v>28</v>
+      </c>
+      <c r="L55" s="33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="B56" s="33">
+        <v>8</v>
+      </c>
+      <c r="C56" s="33">
+        <v>1</v>
+      </c>
+      <c r="D56" s="33">
+        <v>0</v>
+      </c>
+      <c r="E56" s="33">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33">
+        <v>1</v>
+      </c>
+      <c r="G56" s="33">
+        <v>0</v>
+      </c>
+      <c r="H56" s="33">
+        <v>0</v>
+      </c>
+      <c r="I56" s="33">
+        <v>0</v>
+      </c>
+      <c r="J56" s="33">
+        <v>14</v>
+      </c>
+      <c r="K56" s="33">
+        <v>22</v>
+      </c>
+      <c r="L56" s="33">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>457</v>
+      </c>
+      <c r="B57" s="33">
+        <v>3</v>
+      </c>
+      <c r="C57" s="33">
+        <v>1</v>
+      </c>
+      <c r="D57" s="33">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33">
+        <v>0</v>
+      </c>
+      <c r="F57" s="33">
+        <v>2</v>
+      </c>
+      <c r="G57" s="33">
+        <v>1</v>
+      </c>
+      <c r="H57" s="33">
+        <v>0</v>
+      </c>
+      <c r="I57" s="33">
+        <v>0</v>
+      </c>
+      <c r="J57" s="33">
+        <v>14</v>
+      </c>
+      <c r="K57" s="33">
+        <v>18</v>
+      </c>
+      <c r="L57" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>458</v>
+      </c>
+      <c r="B58" s="33">
+        <v>4</v>
+      </c>
+      <c r="C58" s="33">
+        <v>0</v>
+      </c>
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33">
+        <v>0</v>
+      </c>
+      <c r="F58" s="33">
+        <v>1</v>
+      </c>
+      <c r="G58" s="33">
+        <v>0</v>
+      </c>
+      <c r="H58" s="33">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33">
+        <v>0</v>
+      </c>
+      <c r="J58" s="33">
+        <v>20</v>
+      </c>
+      <c r="K58" s="33">
+        <v>25</v>
+      </c>
+      <c r="L58" s="33">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>459</v>
+      </c>
+      <c r="B59" s="33">
+        <v>2</v>
+      </c>
+      <c r="C59" s="33">
+        <v>1</v>
+      </c>
+      <c r="D59" s="33">
+        <v>0</v>
+      </c>
+      <c r="E59" s="33">
+        <v>0</v>
+      </c>
+      <c r="F59" s="33">
+        <v>1</v>
+      </c>
+      <c r="G59" s="33">
+        <v>1</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="33">
+        <v>56</v>
+      </c>
+      <c r="K59" s="33">
+        <v>58</v>
+      </c>
+      <c r="L59" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="37">
+        <v>58</v>
+      </c>
+      <c r="B60" s="37">
+        <f>SUM(B2:B59)</f>
+        <v>365</v>
+      </c>
+      <c r="C60" s="37">
+        <f t="shared" ref="C60:L60" si="0">SUM(C2:C59)</f>
+        <v>25</v>
+      </c>
+      <c r="D60" s="37">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E60" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="37">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="G60" s="37">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="H60" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J60" s="37">
+        <f t="shared" si="0"/>
+        <v>2133</v>
+      </c>
+      <c r="K60" s="37">
+        <f t="shared" si="0"/>
+        <v>2582</v>
+      </c>
+      <c r="L60" s="37">
+        <f t="shared" si="0"/>
+        <v>2942</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="32"/>
+      <c r="E61" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61">
+        <f>G60</f>
+        <v>135</v>
+      </c>
+      <c r="J61">
+        <f>B60-C60</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>107</v>
+      </c>
+      <c r="F62">
+        <f>B60</f>
+        <v>365</v>
+      </c>
+      <c r="J62">
+        <f>D60-E60</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>108</v>
+      </c>
+      <c r="F63">
+        <v>12</v>
+      </c>
+      <c r="J63">
+        <f>F69</f>
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64">
+        <v>8</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F65" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J65">
+        <f>SUM(J61:J64)</f>
+        <v>2942</v>
+      </c>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f>SUM(F61:F65)</f>
+        <v>520</v>
+      </c>
+      <c r="J66" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67">
+        <f>K60-F66</f>
+        <v>2062</v>
+      </c>
+      <c r="J67">
+        <f>J65-L60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F68" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f>F67+F66</f>
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>F69-K60</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17479,7 +20071,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="102" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
@@ -17522,16 +20114,30 @@
       <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="E3" s="11">
+        <v>2388</v>
+      </c>
+      <c r="F3" s="11">
+        <v>2424</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1821</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2243</v>
+      </c>
+      <c r="I3" s="11">
+        <v>2225</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1889</v>
+      </c>
+      <c r="K3" s="11">
+        <v>2062</v>
+      </c>
       <c r="L3" s="11">
         <f>SUM(E3:K3)</f>
-        <v>0</v>
+        <v>15052</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="42.75" x14ac:dyDescent="0.2">
@@ -17544,16 +20150,30 @@
       <c r="D4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="E4" s="11">
+        <v>224</v>
+      </c>
+      <c r="F4" s="11">
+        <v>251</v>
+      </c>
+      <c r="G4" s="11">
+        <v>162</v>
+      </c>
+      <c r="H4" s="11">
+        <v>178</v>
+      </c>
+      <c r="I4" s="11">
+        <v>133</v>
+      </c>
+      <c r="J4" s="11">
+        <v>104</v>
+      </c>
+      <c r="K4" s="11">
+        <v>135</v>
+      </c>
       <c r="L4" s="11">
         <f>SUM(E4:K4)</f>
-        <v>0</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="71.25" x14ac:dyDescent="0.2">
@@ -17566,16 +20186,30 @@
       <c r="D5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="E5" s="11">
+        <v>447</v>
+      </c>
+      <c r="F5" s="11">
+        <v>490</v>
+      </c>
+      <c r="G5" s="11">
+        <v>472</v>
+      </c>
+      <c r="H5" s="11">
+        <v>457</v>
+      </c>
+      <c r="I5" s="11">
+        <v>353</v>
+      </c>
+      <c r="J5" s="11">
+        <v>408</v>
+      </c>
+      <c r="K5" s="11">
+        <v>365</v>
+      </c>
       <c r="L5" s="11">
         <f>SUM(E5:K5)</f>
-        <v>0</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="55.5" x14ac:dyDescent="0.2">
@@ -17588,16 +20222,30 @@
       <c r="D6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="E6" s="11">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11">
+        <v>28</v>
+      </c>
+      <c r="G6" s="11">
+        <v>18</v>
+      </c>
+      <c r="H6" s="11">
+        <v>24</v>
+      </c>
+      <c r="I6" s="11">
+        <v>11</v>
+      </c>
+      <c r="J6" s="11">
+        <v>33</v>
+      </c>
+      <c r="K6" s="11">
+        <v>12</v>
+      </c>
       <c r="L6" s="11">
         <f>SUM(E6:K6)</f>
-        <v>0</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -17610,16 +20258,30 @@
       <c r="D7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="E7" s="11">
+        <v>5</v>
+      </c>
+      <c r="F7" s="11">
+        <v>2</v>
+      </c>
+      <c r="G7" s="11">
+        <v>4</v>
+      </c>
+      <c r="H7" s="11">
+        <v>4</v>
+      </c>
+      <c r="I7" s="11">
+        <v>5</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2</v>
+      </c>
+      <c r="K7" s="11">
+        <v>8</v>
+      </c>
       <c r="L7" s="11">
         <f>SUM(E7:K7)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -17628,16 +20290,37 @@
       <c r="D8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="E8" s="15">
+        <f t="shared" ref="E8:K8" si="0">SUM(E3:E7)</f>
+        <v>3081</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="0"/>
+        <v>3195</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>2477</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="0"/>
+        <v>2906</v>
+      </c>
+      <c r="I8" s="15">
+        <f t="shared" si="0"/>
+        <v>2727</v>
+      </c>
+      <c r="J8" s="15">
+        <f t="shared" si="0"/>
+        <v>2436</v>
+      </c>
+      <c r="K8" s="15">
+        <f t="shared" si="0"/>
+        <v>2582</v>
+      </c>
       <c r="L8" s="15">
-        <f t="shared" ref="L8" si="0">SUM(L3:L7)</f>
-        <v>0</v>
+        <f t="shared" ref="L8" si="1">SUM(L3:L7)</f>
+        <v>19404</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -17719,16 +20402,37 @@
       <c r="D14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
+      <c r="E14" s="11">
+        <f>E3</f>
+        <v>2388</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" ref="F14:K14" si="2">F3</f>
+        <v>2424</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" si="2"/>
+        <v>1821</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="2"/>
+        <v>2243</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="2"/>
+        <v>2225</v>
+      </c>
+      <c r="J14" s="11">
+        <f t="shared" si="2"/>
+        <v>1889</v>
+      </c>
+      <c r="K14" s="11">
+        <f t="shared" si="2"/>
+        <v>2062</v>
+      </c>
       <c r="L14" s="11">
         <f>SUM(E14:K14)</f>
-        <v>0</v>
+        <v>15052</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="57" x14ac:dyDescent="0.3">
@@ -17741,16 +20445,37 @@
       <c r="D15" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="E15" s="11">
+        <f>E4</f>
+        <v>224</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" ref="F15:K15" si="3">F4</f>
+        <v>251</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="3"/>
+        <v>162</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="3"/>
+        <v>178</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="3"/>
+        <v>133</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
       <c r="L15" s="11">
         <f>SUM(E15:K15)</f>
-        <v>0</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -17763,16 +20488,37 @@
       <c r="D16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="E16" s="11">
+        <f>E5</f>
+        <v>447</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" ref="F16:K16" si="4">F5</f>
+        <v>490</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="4"/>
+        <v>472</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="4"/>
+        <v>457</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="4"/>
+        <v>353</v>
+      </c>
+      <c r="J16" s="11">
+        <f t="shared" si="4"/>
+        <v>408</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" si="4"/>
+        <v>365</v>
+      </c>
       <c r="L16" s="11">
         <f>SUM(E16:K16)</f>
-        <v>0</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="85.5" x14ac:dyDescent="0.2">
@@ -17785,16 +20531,37 @@
       <c r="D17" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="E17" s="11">
+        <f>E6</f>
+        <v>17</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" ref="F17:K17" si="5">F6</f>
+        <v>28</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
       <c r="L17" s="11">
         <f>SUM(E17:K17)</f>
-        <v>0</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="85.5" x14ac:dyDescent="0.2">
@@ -17807,16 +20574,37 @@
       <c r="D18" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="E18" s="11">
+        <f>E7</f>
+        <v>5</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" ref="F18:K18" si="6">F7</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="J18" s="11">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K18" s="11">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
       <c r="L18" s="11">
         <f>SUM(E18:K18)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -17825,16 +20613,37 @@
       <c r="D19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="E19" s="15">
+        <f t="shared" ref="E19:K19" si="7">SUM(E14:E18)</f>
+        <v>3081</v>
+      </c>
+      <c r="F19" s="15">
+        <f t="shared" si="7"/>
+        <v>3195</v>
+      </c>
+      <c r="G19" s="15">
+        <f t="shared" si="7"/>
+        <v>2477</v>
+      </c>
+      <c r="H19" s="15">
+        <f t="shared" si="7"/>
+        <v>2906</v>
+      </c>
+      <c r="I19" s="15">
+        <f t="shared" si="7"/>
+        <v>2727</v>
+      </c>
+      <c r="J19" s="15">
+        <f t="shared" si="7"/>
+        <v>2436</v>
+      </c>
+      <c r="K19" s="15">
+        <f t="shared" si="7"/>
+        <v>2582</v>
+      </c>
       <c r="L19" s="15">
-        <f t="shared" ref="L19" si="1">SUM(L14:L18)</f>
-        <v>0</v>
+        <f t="shared" ref="L19" si="8">SUM(L14:L18)</f>
+        <v>19404</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -17916,16 +20725,37 @@
       <c r="D25" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="E25" s="11">
+        <f>E14</f>
+        <v>2388</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" ref="F25:K25" si="9">F14</f>
+        <v>2424</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="9"/>
+        <v>1821</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" si="9"/>
+        <v>2243</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" si="9"/>
+        <v>2225</v>
+      </c>
+      <c r="J25" s="11">
+        <f t="shared" si="9"/>
+        <v>1889</v>
+      </c>
+      <c r="K25" s="11">
+        <f t="shared" si="9"/>
+        <v>2062</v>
+      </c>
       <c r="L25" s="11">
         <f>SUM(E25:K25)</f>
-        <v>0</v>
+        <v>15052</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="82.5" x14ac:dyDescent="0.4">
@@ -17938,16 +20768,37 @@
       <c r="D26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
+      <c r="E26" s="11">
+        <f>E15</f>
+        <v>224</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" ref="F26:K26" si="10">F15</f>
+        <v>251</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="10"/>
+        <v>162</v>
+      </c>
+      <c r="H26" s="11">
+        <f t="shared" si="10"/>
+        <v>178</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="10"/>
+        <v>133</v>
+      </c>
+      <c r="J26" s="11">
+        <f t="shared" si="10"/>
+        <v>104</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="10"/>
+        <v>135</v>
+      </c>
       <c r="L26" s="11">
         <f>SUM(E26:K26)</f>
-        <v>0</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="102" x14ac:dyDescent="0.2">
@@ -17960,16 +20811,37 @@
       <c r="D27" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+      <c r="E27" s="11">
+        <f>E16</f>
+        <v>447</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" ref="F27:K27" si="11">F16</f>
+        <v>490</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="11"/>
+        <v>472</v>
+      </c>
+      <c r="H27" s="11">
+        <f t="shared" si="11"/>
+        <v>457</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" si="11"/>
+        <v>353</v>
+      </c>
+      <c r="J27" s="11">
+        <f t="shared" si="11"/>
+        <v>408</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" si="11"/>
+        <v>365</v>
+      </c>
       <c r="L27" s="11">
         <f>SUM(E27:K27)</f>
-        <v>0</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="89.25" x14ac:dyDescent="0.2">
@@ -17982,16 +20854,37 @@
       <c r="D28" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="E28" s="11">
+        <f>E17</f>
+        <v>17</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" ref="F28:K28" si="12">F17</f>
+        <v>28</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="H28" s="11">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+      <c r="J28" s="11">
+        <f t="shared" si="12"/>
+        <v>33</v>
+      </c>
+      <c r="K28" s="11">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
       <c r="L28" s="11">
         <f>SUM(E28:K28)</f>
-        <v>0</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="132" x14ac:dyDescent="0.4">
@@ -18004,16 +20897,37 @@
       <c r="D29" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="E29" s="11">
+        <f>E18</f>
+        <v>5</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" ref="F29:K29" si="13">F18</f>
+        <v>2</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="H29" s="11">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="J29" s="11">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="K29" s="11">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
       <c r="L29" s="11">
         <f>SUM(E29:K29)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -18022,16 +20936,37 @@
       <c r="D30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
+      <c r="E30" s="15">
+        <f t="shared" ref="E30:K30" si="14">SUM(E25:E29)</f>
+        <v>3081</v>
+      </c>
+      <c r="F30" s="15">
+        <f t="shared" si="14"/>
+        <v>3195</v>
+      </c>
+      <c r="G30" s="15">
+        <f t="shared" si="14"/>
+        <v>2477</v>
+      </c>
+      <c r="H30" s="15">
+        <f t="shared" si="14"/>
+        <v>2906</v>
+      </c>
+      <c r="I30" s="15">
+        <f t="shared" si="14"/>
+        <v>2727</v>
+      </c>
+      <c r="J30" s="15">
+        <f t="shared" si="14"/>
+        <v>2436</v>
+      </c>
+      <c r="K30" s="15">
+        <f t="shared" si="14"/>
+        <v>2582</v>
+      </c>
       <c r="L30" s="15">
-        <f t="shared" ref="L30" si="2">SUM(L25:L29)</f>
-        <v>0</v>
+        <f t="shared" ref="L30" si="15">SUM(L25:L29)</f>
+        <v>19404</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">

</xml_diff>